<commit_message>
Created board layout, added info
</commit_message>
<xml_diff>
--- a/DOCS/MOSFET comparison.xlsx
+++ b/DOCS/MOSFET comparison.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47157143-5F83-4871-812F-2A607CE86D52}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA4BAF71-8113-4913-8BCA-8BBA3847C4DF}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="594" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -784,7 +784,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -862,6 +862,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3306,247 +3309,247 @@
                   <c:v>39.466477977598117</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="0.0">
-                  <c:v>36.95983304356885</c:v>
+                  <c:v>43.269076398215475</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="0.0">
-                  <c:v>33.790454220571526</c:v>
+                  <c:v>46.92853011606438</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="0.0">
-                  <c:v>31.121706317367202</c:v>
+                  <c:v>50.354147410673434</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="0.0">
-                  <c:v>28.843653490082446</c:v>
+                  <c:v>51.823341619826913</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="0.0">
-                  <c:v>26.876352884777766</c:v>
+                  <c:v>48.288696073878597</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="0.0">
-                  <c:v>25.160279272291959</c:v>
+                  <c:v>45.205429625153542</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="0.0">
-                  <c:v>23.650197875524661</c:v>
+                  <c:v>42.492269028999353</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="0.0">
-                  <c:v>22.324623266371834</c:v>
+                  <c:v>40.110611454437382</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="0.0">
-                  <c:v>21.115551771799847</c:v>
+                  <c:v>37.938274821439656</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="0.0">
-                  <c:v>20.041599608132401</c:v>
+                  <c:v>36.008706853213063</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0.0">
-                  <c:v>19.071604094708277</c:v>
+                  <c:v>34.265917616088096</c:v>
                 </c:pt>
                 <c:pt idx="22" formatCode="0.0">
-                  <c:v>18.191167826131544</c:v>
+                  <c:v>32.68403931704993</c:v>
                 </c:pt>
                 <c:pt idx="23" formatCode="0.0">
-                  <c:v>17.388434690558867</c:v>
+                  <c:v>31.241770100751051</c:v>
                 </c:pt>
                 <c:pt idx="24" formatCode="0.0">
-                  <c:v>16.65355286033369</c:v>
+                  <c:v>29.921409205725816</c:v>
                 </c:pt>
                 <c:pt idx="25" formatCode="0.0">
-                  <c:v>15.978268433682603</c:v>
+                  <c:v>28.708126861139302</c:v>
                 </c:pt>
                 <c:pt idx="26" formatCode="0.0">
-                  <c:v>15.355614088245334</c:v>
+                  <c:v>27.589404891130879</c:v>
                 </c:pt>
                 <c:pt idx="27" formatCode="0.0">
-                  <c:v>14.779667801034744</c:v>
+                  <c:v>26.554603207389672</c:v>
                 </c:pt>
                 <c:pt idx="28" formatCode="0.0">
-                  <c:v>14.245363903889437</c:v>
+                  <c:v>25.59462033281774</c:v>
                 </c:pt>
                 <c:pt idx="29" formatCode="0.0">
-                  <c:v>13.748343692535274</c:v>
+                  <c:v>24.701624991093023</c:v>
                 </c:pt>
                 <c:pt idx="30" formatCode="0.0">
-                  <c:v>13.284836254768264</c:v>
+                  <c:v>23.868841990874635</c:v>
                 </c:pt>
                 <c:pt idx="31" formatCode="0.0">
-                  <c:v>12.851562618762276</c:v>
+                  <c:v>23.090380009235478</c:v>
                 </c:pt>
                 <c:pt idx="32" formatCode="0.0">
-                  <c:v>12.445658065691552</c:v>
+                  <c:v>22.361092010887415</c:v>
                 </c:pt>
                 <c:pt idx="33" formatCode="0.0">
-                  <c:v>12.064608713703821</c:v>
+                  <c:v>21.676461308717052</c:v>
                 </c:pt>
                 <c:pt idx="34" formatCode="0.0">
-                  <c:v>11.706199405481359</c:v>
+                  <c:v>21.032507933458092</c:v>
                 </c:pt>
                 <c:pt idx="35" formatCode="0.0">
-                  <c:v>11.419154836911821</c:v>
+                  <c:v>20.516775460725057</c:v>
                 </c:pt>
                 <c:pt idx="36" formatCode="0.0">
-                  <c:v>8.8088207945727248</c:v>
+                  <c:v>15.826792866650564</c:v>
                 </c:pt>
                 <c:pt idx="37" formatCode="0.0">
-                  <c:v>8.1384569896295247</c:v>
+                  <c:v>14.622351394453444</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>7.5350960974362318</c:v>
+                  <c:v>13.538293938038368</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>6.9764665795921719</c:v>
+                  <c:v>12.534605263435964</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>6.459252185612673</c:v>
+                  <c:v>11.605327069218733</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>5.9803825219185756</c:v>
+                  <c:v>10.744942784629968</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>5.5370148247396225</c:v>
+                  <c:v>9.9483448209912382</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>5.126517084320346</c:v>
+                  <c:v>9.2108042509927159</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>4.7464524202469009</c:v>
+                  <c:v>8.5279427358703277</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>4.3945646151405482</c:v>
+                  <c:v>7.8957065338181902</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>4.0687647208398232</c:v>
+                  <c:v>7.310342435339634</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>3.767118657560415</c:v>
+                  <c:v>6.7683754826795051</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>3.487835732416257</c:v>
+                  <c:v>6.2665883410711523</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>3.2292580091431691</c:v>
+                  <c:v>5.8020021993375517</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>2.9898504659194685</c:v>
+                  <c:v>5.3718590864648608</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>2.7681918828563123</c:v>
+                  <c:v>4.973605499172308</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>2.5629664050623386</c:v>
+                  <c:v>4.6048772432852303</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>2.3729557311974583</c:v>
+                  <c:v>4.2634853989233852</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>2.1970318811439506</c:v>
+                  <c:v>3.9474033261882897</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>2.03415049986083</c:v>
+                  <c:v>3.6547546342101116</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>1.8833446576704247</c:v>
+                  <c:v>3.3838020421334432</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>1.7437191101732159</c:v>
+                  <c:v>3.1329370659163636</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>1.6144449837154315</c:v>
+                  <c:v>2.9006704697193877</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>1.4947548548601968</c:v>
+                  <c:v>2.6856234251999176</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>1.3839381946520117</c:v>
+                  <c:v>2.4865193262302197</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>1.2813371506298283</c:v>
+                  <c:v>2.3021762104477217</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>1.1863426415491065</c:v>
+                  <c:v>2.1314997426489843</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>1.0983907416294878</c:v>
+                  <c:v>1.9734767183738373</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>1.0169593328635618</c:v>
+                  <c:v>1.8271690491144155</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.94156500551345956</c:v>
+                  <c:v>1.6917081934428257</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.8777965868394163</c:v>
+                  <c:v>1.5771355874920097</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.81493958561453539</c:v>
+                  <c:v>1.464200523673034</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.75452239890622275</c:v>
+                  <c:v>1.3556490703153545</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.69858436195843443</c:v>
+                  <c:v>1.2551452974738009</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.64679340398684038</c:v>
+                  <c:v>1.1620925741527808</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.5988420729431897</c:v>
+                  <c:v>1.0759385017966225</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.55444571035574841</c:v>
+                  <c:v>0.99617163502859096</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.51334076148162311</c:v>
+                  <c:v>0.92231844550453301</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.47528321073933727</c:v>
+                  <c:v>0.85394051085733169</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.44004713313376675</c:v>
+                  <c:v>0.79063191204463001</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>0.40742335307410504</c:v>
+                  <c:v>0.73201682364942156</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.37721820262305267</c:v>
+                  <c:v>0.67774728282854824</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>0.34925237180571045</c:v>
+                  <c:v>0.62750112366470556</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.32335984415312985</c:v>
+                  <c:v>0.58098006465940732</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.29794903266040068</c:v>
+                  <c:v>0.53532450423334965</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.27719125981633252</c:v>
+                  <c:v>0.49802905018364718</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.25664112776500114</c:v>
+                  <c:v>0.46110666398195194</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.23761452112210815</c:v>
+                  <c:v>0.42692159320859291</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>0.21999849026453824</c:v>
+                  <c:v>0.39527090147388755</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>0.203688459316862</c:v>
+                  <c:v>0.36596669748592875</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>0.18858760534669269</c:v>
+                  <c:v>0.33883501965197188</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>0.17460628358464719</c:v>
+                  <c:v>0.31371480337214674</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>0.16166149525678214</c:v>
+                  <c:v>0.29045692489492958</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>0.14967639487034218</c:v>
+                  <c:v>0.26892331605831116</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>0.14025782871073497</c:v>
+                  <c:v>0.25200099476409327</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>0.13791427064949893</c:v>
+                  <c:v>0.22422064894203664</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3914,244 +3917,244 @@
                   <c:v>43.269076398215475</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="0.0">
-                  <c:v>43.215182987536537</c:v>
+                  <c:v>46.92853011606438</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="0.0">
-                  <c:v>39.802076190221975</c:v>
+                  <c:v>50.354147410673434</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="0.0">
-                  <c:v>36.888635928550322</c:v>
+                  <c:v>53.89215007900944</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="0.0">
-                  <c:v>34.372621935522233</c:v>
+                  <c:v>57.280946563595151</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="0.0">
-                  <c:v>32.177906389540951</c:v>
+                  <c:v>60.50949774343708</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="0.0">
-                  <c:v>30.24663776967007</c:v>
+                  <c:v>63.808129536553629</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="0.0">
-                  <c:v>28.551337998786941</c:v>
+                  <c:v>65.953934522002655</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="0.0">
-                  <c:v>27.005036030134121</c:v>
+                  <c:v>62.381958357659499</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="0.0">
-                  <c:v>25.631540457396468</c:v>
+                  <c:v>59.209167048388856</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0.0">
-                  <c:v>24.390996801602899</c:v>
+                  <c:v>56.343496267938185</c:v>
                 </c:pt>
                 <c:pt idx="22" formatCode="0.0">
-                  <c:v>23.264991977665261</c:v>
+                  <c:v>53.742411568068867</c:v>
                 </c:pt>
                 <c:pt idx="23" formatCode="0.0">
-                  <c:v>22.238363003769642</c:v>
+                  <c:v>51.370886278235545</c:v>
                 </c:pt>
                 <c:pt idx="24" formatCode="0.0">
-                  <c:v>21.298510211022556</c:v>
+                  <c:v>49.199815011600116</c:v>
                 </c:pt>
                 <c:pt idx="25" formatCode="0.0">
-                  <c:v>20.434877544948652</c:v>
+                  <c:v>47.20481315523454</c:v>
                 </c:pt>
                 <c:pt idx="26" formatCode="0.0">
-                  <c:v>19.638554379228232</c:v>
+                  <c:v>45.365297055060537</c:v>
                 </c:pt>
                 <c:pt idx="27" formatCode="0.0">
-                  <c:v>18.901966938576276</c:v>
+                  <c:v>43.663771198984982</c:v>
                 </c:pt>
                 <c:pt idx="28" formatCode="0.0">
-                  <c:v>18.218636654367454</c:v>
+                  <c:v>42.085270015484404</c:v>
                 </c:pt>
                 <c:pt idx="29" formatCode="0.0">
-                  <c:v>17.582989106040092</c:v>
+                  <c:v>40.616916525947921</c:v>
                 </c:pt>
                 <c:pt idx="30" formatCode="0.0">
-                  <c:v>16.990201610245169</c:v>
+                  <c:v>39.247570273776432</c:v>
                 </c:pt>
                 <c:pt idx="31" formatCode="0.0">
-                  <c:v>16.436080634497085</c:v>
+                  <c:v>37.967544148440027</c:v>
                 </c:pt>
                 <c:pt idx="32" formatCode="0.0">
-                  <c:v>15.91696244147361</c:v>
+                  <c:v>36.768374872614658</c:v>
                 </c:pt>
                 <c:pt idx="33" formatCode="0.0">
-                  <c:v>15.429631985187322</c:v>
+                  <c:v>35.642635651361736</c:v>
                 </c:pt>
                 <c:pt idx="34" formatCode="0.0">
-                  <c:v>14.971256263506714</c:v>
+                  <c:v>34.583782215649443</c:v>
                 </c:pt>
                 <c:pt idx="35" formatCode="0.0">
-                  <c:v>14.604150113487602</c:v>
+                  <c:v>33.735762589318313</c:v>
                 </c:pt>
                 <c:pt idx="36" formatCode="0.0">
-                  <c:v>11.265749790073068</c:v>
+                  <c:v>26.02401764944651</c:v>
                 </c:pt>
                 <c:pt idx="37" formatCode="0.0">
-                  <c:v>10.408410190263698</c:v>
+                  <c:v>24.0435528519176</c:v>
                 </c:pt>
                 <c:pt idx="38" formatCode="0.0">
-                  <c:v>9.6367617479713044</c:v>
+                  <c:v>22.261035659934503</c:v>
                 </c:pt>
                 <c:pt idx="39" formatCode="0.0">
-                  <c:v>8.9223210163290165</c:v>
+                  <c:v>20.610668968307333</c:v>
                 </c:pt>
                 <c:pt idx="40" formatCode="0.0">
-                  <c:v>8.2608467865447857</c:v>
+                  <c:v>19.082655533664276</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>7.6484122803781949</c:v>
+                  <c:v>17.667924450993389</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>7.0813818391985546</c:v>
+                  <c:v>16.358077305086137</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>6.5563893412465903</c:v>
+                  <c:v>15.145338314152067</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>6.0703182189758715</c:v>
+                  <c:v>14.022508169636902</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>5.6202829578489082</c:v>
+                  <c:v>12.982921298218784</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>5.2036119667571601</c:v>
+                  <c:v>12.020406292272279</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>4.8178317183770254</c:v>
+                  <c:v>11.129249273899747</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>4.4606520653124173</c:v>
+                  <c:v>10.304159975043921</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>4.1299526448546686</c:v>
+                  <c:v>9.5402403323196054</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>3.8237702916529721</c:v>
+                  <c:v>8.8329554101308307</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>3.5402873835717701</c:v>
+                  <c:v>8.1781064794611424</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>3.2778210515515314</c:v>
+                  <c:v>7.5718060925220607</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>3.0348131894181813</c:v>
+                  <c:v>7.0104550052926013</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>2.8098212043354285</c:v>
+                  <c:v>6.4907208109527863</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>2.6015094529909475</c:v>
+                  <c:v>6.0095181573706205</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>2.4086413126781032</c:v>
+                  <c:v>5.5639904312054158</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>2.2300718402040283</c:v>
+                  <c:v>5.1514927998970652</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>2.0647409750443053</c:v>
+                  <c:v>4.7695765108715324</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>1.9116672463954658</c:v>
+                  <c:v>4.4159743547563517</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>1.7699419467678312</c:v>
+                  <c:v>4.0885872063099509</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>1.6387237375307506</c:v>
+                  <c:v>3.7854715631662019</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>1.5172336543866372</c:v>
+                  <c:v>3.5048280084193122</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>1.4047504831242079</c:v>
+                  <c:v>3.2449905285581346</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>1.300606478199587</c:v>
+                  <c:v>3.0044166233369713</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>1.2041833987290149</c:v>
+                  <c:v>2.7816781488710052</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>1.1226288903511155</c:v>
+                  <c:v>2.5932862526397806</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>1.0422400091526107</c:v>
+                  <c:v>2.4075869692265659</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.96497144797410017</c:v>
+                  <c:v>2.2290956626267362</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.89343134712542449</c:v>
+                  <c:v>2.0638371683568182</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.82719501566825004</c:v>
+                  <c:v>1.91083044523618</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.76586924798189138</c:v>
+                  <c:v>1.769167183547026</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.7090899895358993</c:v>
+                  <c:v>1.6380064129409713</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.65652017571530796</c:v>
+                  <c:v>1.5165695100993439</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.60784773086891486</c:v>
+                  <c:v>1.4041355765106209</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.56278371570214825</c:v>
+                  <c:v>1.300037158925647</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>0.52106061201669618</c:v>
+                  <c:v>1.203656287085527</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.48243073461440833</c:v>
+                  <c:v>1.1144208052005193</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>0.44666476093790852</c:v>
+                  <c:v>1.0318009754021482</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.41355036971925169</c:v>
+                  <c:v>0.95530633300521173</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.38105205343880499</c:v>
+                  <c:v>0.86429450919459005</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.35450458692608788</c:v>
+                  <c:v>0.76337281522955247</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.32822267573249214</c:v>
+                  <c:v>0.6794182695875215</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.30388922693250758</c:v>
+                  <c:v>0.60469691327754749</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>0.28135978734419603</c:v>
+                  <c:v>0.53840446288357602</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>0.26050061311305744</c:v>
+                  <c:v>0.47900363967956822</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>0.24118787575447997</c:v>
+                  <c:v>0.42632357021955675</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>0.22330692705783342</c:v>
+                  <c:v>0.37958605013304503</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>0.20675161848837811</c:v>
+                  <c:v>0.33923104342632693</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>0.19142367104668084</c:v>
+                  <c:v>0.31125786554921364</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>0.17937810760409625</c:v>
+                  <c:v>0.28067652277033595</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>0.17638089159163514</c:v>
+                  <c:v>0.22422064894203664</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5975,51 +5978,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="I1" s="27" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="I1" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="Q1" s="27" t="s">
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="Q1" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="27"/>
-      <c r="W1" s="27"/>
-      <c r="Y1" s="27" t="s">
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
+      <c r="Y1" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="Z1" s="27"/>
-      <c r="AA1" s="27"/>
-      <c r="AB1" s="27"/>
-      <c r="AC1" s="27"/>
-      <c r="AD1" s="27"/>
-      <c r="AE1" s="27"/>
-      <c r="AG1" s="27" t="s">
+      <c r="Z1" s="28"/>
+      <c r="AA1" s="28"/>
+      <c r="AB1" s="28"/>
+      <c r="AC1" s="28"/>
+      <c r="AD1" s="28"/>
+      <c r="AE1" s="28"/>
+      <c r="AG1" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="AH1" s="27"/>
-      <c r="AI1" s="27"/>
-      <c r="AJ1" s="27"/>
-      <c r="AK1" s="27"/>
-      <c r="AL1" s="27"/>
-      <c r="AM1" s="27"/>
+      <c r="AH1" s="28"/>
+      <c r="AI1" s="28"/>
+      <c r="AJ1" s="28"/>
+      <c r="AK1" s="28"/>
+      <c r="AL1" s="28"/>
+      <c r="AM1" s="28"/>
     </row>
     <row r="2" spans="1:39" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -8893,7 +8896,7 @@
   <dimension ref="A1:M98"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.7109375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8907,19 +8910,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28" t="s">
+      <c r="E1" s="29"/>
+      <c r="F1" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="28"/>
+      <c r="G1" s="29"/>
     </row>
     <row r="2" spans="1:13" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="24" t="s">
@@ -9074,15 +9077,15 @@
       <c r="J5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="K5" s="7">
-        <v>0.4</v>
+      <c r="K5" s="27">
+        <v>0.16948353896707699</v>
       </c>
       <c r="L5" s="3" t="s">
         <v>7</v>
       </c>
       <c r="M5" s="12">
         <f>M7+K6*K10</f>
-        <v>114.13180886168902</v>
+        <v>105.47314004989263</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9119,14 +9122,14 @@
         <v>23</v>
       </c>
       <c r="K6" s="2">
-        <v>0.579639580109088</v>
+        <v>9.0038130076260103E-2</v>
       </c>
       <c r="L6" s="3" t="s">
         <v>7</v>
       </c>
       <c r="M6" s="12">
         <f>M8+K6*K11</f>
-        <v>111.10048667236624</v>
+        <v>92.891956869502621</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9170,7 +9173,7 @@
       </c>
       <c r="M7" s="12">
         <f>K2+K7*K10</f>
-        <v>61.634860962056614</v>
+        <v>90.821790415153615</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9214,7 +9217,7 @@
       </c>
       <c r="M8" s="12">
         <f>K2+K8*K11</f>
-        <v>43.961252764447053</v>
+        <v>68.800722170520174</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9277,7 +9280,7 @@
       </c>
       <c r="K10" s="9">
         <f>($K$3-$K$2)/(SUM(K7,K6,K4))</f>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="L10" s="8" t="s">
         <v>3</v>
@@ -9315,7 +9318,7 @@
       </c>
       <c r="K11" s="9">
         <f>($K$3-$K$2)/(SUM(K8,K6,K4))</f>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
       <c r="L11" s="8" t="s">
         <v>3</v>
@@ -9353,7 +9356,7 @@
       </c>
       <c r="K12" s="12">
         <f>MAX(D3:D94)</f>
-        <v>39.466477977598117</v>
+        <v>51.823341619826913</v>
       </c>
       <c r="L12" s="8" t="s">
         <v>42</v>
@@ -9391,7 +9394,7 @@
       </c>
       <c r="K13" s="12">
         <f>MAX(F3:F94)</f>
-        <v>43.269076398215475</v>
+        <v>65.953934522002655</v>
       </c>
       <c r="L13" s="8" t="s">
         <v>42</v>
@@ -9410,11 +9413,11 @@
       </c>
       <c r="D14" s="18">
         <f t="shared" si="0"/>
-        <v>36.95983304356885</v>
+        <v>43.269076398215475</v>
       </c>
       <c r="E14" s="17">
         <f t="shared" si="1"/>
-        <v>90.56825948592487</v>
+        <v>106.02875111287261</v>
       </c>
       <c r="F14" s="18">
         <f t="shared" si="2"/>
@@ -9422,7 +9425,7 @@
       </c>
       <c r="G14" s="17">
         <f t="shared" si="3"/>
-        <v>115.82927773028129</v>
+        <v>106.02875111287261</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9438,19 +9441,19 @@
       </c>
       <c r="D15" s="18">
         <f t="shared" si="0"/>
-        <v>33.790454220571526</v>
+        <v>46.92853011606438</v>
       </c>
       <c r="E15" s="17">
         <f t="shared" si="1"/>
-        <v>90.56825948592487</v>
+        <v>125.78212962456209</v>
       </c>
       <c r="F15" s="18">
         <f t="shared" si="2"/>
-        <v>43.215182987536537</v>
+        <v>46.92853011606438</v>
       </c>
       <c r="G15" s="17">
         <f t="shared" si="3"/>
-        <v>115.82927773028129</v>
+        <v>125.78212962456209</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9466,19 +9469,19 @@
       </c>
       <c r="D16" s="18">
         <f t="shared" si="0"/>
-        <v>31.121706317367202</v>
+        <v>50.354147410673434</v>
       </c>
       <c r="E16" s="17">
         <f t="shared" si="1"/>
-        <v>90.56825948592487</v>
+        <v>146.53719312097749</v>
       </c>
       <c r="F16" s="18">
         <f t="shared" si="2"/>
-        <v>39.802076190221975</v>
+        <v>50.354147410673434</v>
       </c>
       <c r="G16" s="17">
         <f t="shared" si="3"/>
-        <v>115.82927773028129</v>
+        <v>146.53719312097749</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9494,19 +9497,19 @@
       </c>
       <c r="D17" s="18">
         <f t="shared" si="0"/>
-        <v>28.843653490082446</v>
+        <v>51.823341619826913</v>
       </c>
       <c r="E17" s="17">
         <f t="shared" si="1"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F17" s="18">
         <f t="shared" si="2"/>
-        <v>36.888635928550322</v>
+        <v>53.89215007900944</v>
       </c>
       <c r="G17" s="17">
         <f t="shared" si="3"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9522,19 +9525,19 @@
       </c>
       <c r="D18" s="18">
         <f t="shared" si="0"/>
-        <v>26.876352884777766</v>
+        <v>48.288696073878597</v>
       </c>
       <c r="E18" s="17">
         <f t="shared" si="1"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F18" s="18">
         <f t="shared" si="2"/>
-        <v>34.372621935522233</v>
+        <v>57.280946563595151</v>
       </c>
       <c r="G18" s="17">
         <f t="shared" si="3"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9550,19 +9553,19 @@
       </c>
       <c r="D19" s="18">
         <f t="shared" si="0"/>
-        <v>25.160279272291959</v>
+        <v>45.205429625153542</v>
       </c>
       <c r="E19" s="17">
         <f t="shared" si="1"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F19" s="18">
         <f t="shared" si="2"/>
-        <v>32.177906389540951</v>
+        <v>60.50949774343708</v>
       </c>
       <c r="G19" s="17">
         <f t="shared" si="3"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9578,19 +9581,19 @@
       </c>
       <c r="D20" s="18">
         <f t="shared" si="0"/>
-        <v>23.650197875524661</v>
+        <v>42.492269028999353</v>
       </c>
       <c r="E20" s="17">
         <f t="shared" si="1"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F20" s="18">
         <f t="shared" si="2"/>
-        <v>30.24663776967007</v>
+        <v>63.808129536553629</v>
       </c>
       <c r="G20" s="17">
         <f t="shared" si="3"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9606,19 +9609,19 @@
       </c>
       <c r="D21" s="18">
         <f t="shared" si="0"/>
-        <v>22.324623266371834</v>
+        <v>40.110611454437382</v>
       </c>
       <c r="E21" s="17">
         <f t="shared" si="1"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F21" s="18">
         <f t="shared" si="2"/>
-        <v>28.551337998786941</v>
+        <v>65.953934522002655</v>
       </c>
       <c r="G21" s="17">
         <f t="shared" si="3"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9634,19 +9637,19 @@
       </c>
       <c r="D22" s="18">
         <f t="shared" si="0"/>
-        <v>21.115551771799847</v>
+        <v>37.938274821439656</v>
       </c>
       <c r="E22" s="17">
         <f t="shared" si="1"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F22" s="18">
         <f t="shared" si="2"/>
-        <v>27.005036030134121</v>
+        <v>62.381958357659499</v>
       </c>
       <c r="G22" s="17">
         <f t="shared" si="3"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9662,19 +9665,19 @@
       </c>
       <c r="D23" s="18">
         <f t="shared" si="0"/>
-        <v>20.041599608132401</v>
+        <v>36.008706853213063</v>
       </c>
       <c r="E23" s="17">
         <f t="shared" si="1"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F23" s="18">
         <f t="shared" si="2"/>
-        <v>25.631540457396468</v>
+        <v>59.209167048388856</v>
       </c>
       <c r="G23" s="17">
         <f t="shared" si="3"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9690,19 +9693,19 @@
       </c>
       <c r="D24" s="18">
         <f t="shared" si="0"/>
-        <v>19.071604094708277</v>
+        <v>34.265917616088096</v>
       </c>
       <c r="E24" s="17">
         <f t="shared" si="1"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F24" s="18">
         <f t="shared" si="2"/>
-        <v>24.390996801602899</v>
+        <v>56.343496267938185</v>
       </c>
       <c r="G24" s="17">
         <f t="shared" si="3"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9718,19 +9721,19 @@
       </c>
       <c r="D25" s="18">
         <f t="shared" si="0"/>
-        <v>18.191167826131544</v>
+        <v>32.68403931704993</v>
       </c>
       <c r="E25" s="17">
         <f t="shared" si="1"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F25" s="18">
         <f t="shared" si="2"/>
-        <v>23.264991977665261</v>
+        <v>53.742411568068867</v>
       </c>
       <c r="G25" s="17">
         <f t="shared" si="3"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9746,19 +9749,19 @@
       </c>
       <c r="D26" s="18">
         <f t="shared" si="0"/>
-        <v>17.388434690558867</v>
+        <v>31.241770100751051</v>
       </c>
       <c r="E26" s="17">
         <f t="shared" si="1"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F26" s="18">
         <f t="shared" si="2"/>
-        <v>22.238363003769642</v>
+        <v>51.370886278235545</v>
       </c>
       <c r="G26" s="17">
         <f t="shared" si="3"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9774,19 +9777,19 @@
       </c>
       <c r="D27" s="18">
         <f t="shared" si="0"/>
-        <v>16.65355286033369</v>
+        <v>29.921409205725816</v>
       </c>
       <c r="E27" s="17">
         <f t="shared" si="1"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F27" s="18">
         <f t="shared" si="2"/>
-        <v>21.298510211022556</v>
+        <v>49.199815011600116</v>
       </c>
       <c r="G27" s="17">
         <f t="shared" si="3"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9802,19 +9805,19 @@
       </c>
       <c r="D28" s="18">
         <f t="shared" si="0"/>
-        <v>15.978268433682603</v>
+        <v>28.708126861139302</v>
       </c>
       <c r="E28" s="17">
         <f t="shared" si="1"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F28" s="18">
         <f t="shared" si="2"/>
-        <v>20.434877544948652</v>
+        <v>47.20481315523454</v>
       </c>
       <c r="G28" s="17">
         <f t="shared" si="3"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9830,19 +9833,19 @@
       </c>
       <c r="D29" s="18">
         <f t="shared" si="0"/>
-        <v>15.355614088245334</v>
+        <v>27.589404891130879</v>
       </c>
       <c r="E29" s="17">
         <f t="shared" si="1"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F29" s="18">
         <f t="shared" si="2"/>
-        <v>19.638554379228232</v>
+        <v>45.365297055060537</v>
       </c>
       <c r="G29" s="17">
         <f t="shared" si="3"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9858,19 +9861,19 @@
       </c>
       <c r="D30" s="18">
         <f t="shared" si="0"/>
-        <v>14.779667801034744</v>
+        <v>26.554603207389672</v>
       </c>
       <c r="E30" s="17">
         <f t="shared" si="1"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F30" s="18">
         <f t="shared" si="2"/>
-        <v>18.901966938576276</v>
+        <v>43.663771198984982</v>
       </c>
       <c r="G30" s="17">
         <f t="shared" si="3"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9886,19 +9889,19 @@
       </c>
       <c r="D31" s="18">
         <f t="shared" si="0"/>
-        <v>14.245363903889437</v>
+        <v>25.59462033281774</v>
       </c>
       <c r="E31" s="17">
         <f t="shared" si="1"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F31" s="18">
         <f t="shared" si="2"/>
-        <v>18.218636654367454</v>
+        <v>42.085270015484404</v>
       </c>
       <c r="G31" s="17">
         <f t="shared" si="3"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9914,19 +9917,19 @@
       </c>
       <c r="D32" s="18">
         <f t="shared" si="0"/>
-        <v>13.748343692535274</v>
+        <v>24.701624991093023</v>
       </c>
       <c r="E32" s="17">
         <f t="shared" si="1"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F32" s="18">
         <f t="shared" si="2"/>
-        <v>17.582989106040092</v>
+        <v>40.616916525947921</v>
       </c>
       <c r="G32" s="17">
         <f t="shared" si="3"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9942,19 +9945,19 @@
       </c>
       <c r="D33" s="18">
         <f t="shared" si="0"/>
-        <v>13.284836254768264</v>
+        <v>23.868841990874635</v>
       </c>
       <c r="E33" s="17">
         <f t="shared" si="1"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F33" s="18">
         <f t="shared" si="2"/>
-        <v>16.990201610245169</v>
+        <v>39.247570273776432</v>
       </c>
       <c r="G33" s="17">
         <f t="shared" si="3"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9970,19 +9973,19 @@
       </c>
       <c r="D34" s="18">
         <f t="shared" si="0"/>
-        <v>12.851562618762276</v>
+        <v>23.090380009235478</v>
       </c>
       <c r="E34" s="17">
         <f t="shared" si="1"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F34" s="18">
         <f t="shared" si="2"/>
-        <v>16.436080634497085</v>
+        <v>37.967544148440027</v>
       </c>
       <c r="G34" s="17">
         <f t="shared" si="3"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9998,19 +10001,19 @@
       </c>
       <c r="D35" s="18">
         <f t="shared" ref="D35:D66" si="5">IF($B35&lt;$K$10/$A35,$B35,$K$10/$A35)</f>
-        <v>12.445658065691552</v>
+        <v>22.361092010887415</v>
       </c>
       <c r="E35" s="17">
         <f t="shared" ref="E35:E66" si="6">IF($D35=$B35,$C35,$K$10)</f>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F35" s="18">
         <f t="shared" ref="F35:F66" si="7">IF($B35&lt;$K$11/$A35,$B35,$K$11/$A35)</f>
-        <v>15.91696244147361</v>
+        <v>36.768374872614658</v>
       </c>
       <c r="G35" s="17">
         <f t="shared" ref="G35:G66" si="8">IF($D35=$B35,$C35,$K$11)</f>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10026,19 +10029,19 @@
       </c>
       <c r="D36" s="18">
         <f t="shared" si="5"/>
-        <v>12.064608713703821</v>
+        <v>21.676461308717052</v>
       </c>
       <c r="E36" s="17">
         <f t="shared" si="6"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F36" s="18">
         <f t="shared" si="7"/>
-        <v>15.429631985187322</v>
+        <v>35.642635651361736</v>
       </c>
       <c r="G36" s="17">
         <f t="shared" si="8"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10054,19 +10057,19 @@
       </c>
       <c r="D37" s="18">
         <f t="shared" si="5"/>
-        <v>11.706199405481359</v>
+        <v>21.032507933458092</v>
       </c>
       <c r="E37" s="17">
         <f t="shared" si="6"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F37" s="18">
         <f t="shared" si="7"/>
-        <v>14.971256263506714</v>
+        <v>34.583782215649443</v>
       </c>
       <c r="G37" s="17">
         <f t="shared" si="8"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10082,19 +10085,19 @@
       </c>
       <c r="D38" s="18">
         <f t="shared" si="5"/>
-        <v>11.419154836911821</v>
+        <v>20.516775460725057</v>
       </c>
       <c r="E38" s="17">
         <f t="shared" si="6"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F38" s="18">
         <f t="shared" si="7"/>
-        <v>14.604150113487602</v>
+        <v>33.735762589318313</v>
       </c>
       <c r="G38" s="17">
         <f t="shared" si="8"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10110,19 +10113,19 @@
       </c>
       <c r="D39" s="18">
         <f t="shared" si="5"/>
-        <v>8.8088207945727248</v>
+        <v>15.826792866650564</v>
       </c>
       <c r="E39" s="17">
         <f t="shared" si="6"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F39" s="18">
         <f t="shared" si="7"/>
-        <v>11.265749790073068</v>
+        <v>26.02401764944651</v>
       </c>
       <c r="G39" s="17">
         <f t="shared" si="8"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10138,19 +10141,19 @@
       </c>
       <c r="D40" s="18">
         <f t="shared" si="5"/>
-        <v>8.1384569896295247</v>
+        <v>14.622351394453444</v>
       </c>
       <c r="E40" s="17">
         <f t="shared" si="6"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F40" s="18">
         <f t="shared" si="7"/>
-        <v>10.408410190263698</v>
+        <v>24.0435528519176</v>
       </c>
       <c r="G40" s="17">
         <f t="shared" si="8"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10166,19 +10169,19 @@
       </c>
       <c r="D41" s="22">
         <f t="shared" si="5"/>
-        <v>7.5350960974362318</v>
+        <v>13.538293938038368</v>
       </c>
       <c r="E41" s="17">
         <f t="shared" si="6"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F41" s="18">
         <f t="shared" si="7"/>
-        <v>9.6367617479713044</v>
+        <v>22.261035659934503</v>
       </c>
       <c r="G41" s="17">
         <f t="shared" si="8"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10194,19 +10197,19 @@
       </c>
       <c r="D42" s="22">
         <f t="shared" si="5"/>
-        <v>6.9764665795921719</v>
+        <v>12.534605263435964</v>
       </c>
       <c r="E42" s="17">
         <f t="shared" si="6"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F42" s="18">
         <f t="shared" si="7"/>
-        <v>8.9223210163290165</v>
+        <v>20.610668968307333</v>
       </c>
       <c r="G42" s="17">
         <f t="shared" si="8"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10222,19 +10225,19 @@
       </c>
       <c r="D43" s="22">
         <f t="shared" si="5"/>
-        <v>6.459252185612673</v>
+        <v>11.605327069218733</v>
       </c>
       <c r="E43" s="17">
         <f t="shared" si="6"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F43" s="18">
         <f t="shared" si="7"/>
-        <v>8.2608467865447857</v>
+        <v>19.082655533664276</v>
       </c>
       <c r="G43" s="17">
         <f t="shared" si="8"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10250,19 +10253,19 @@
       </c>
       <c r="D44" s="22">
         <f t="shared" si="5"/>
-        <v>5.9803825219185756</v>
+        <v>10.744942784629968</v>
       </c>
       <c r="E44" s="17">
         <f t="shared" si="6"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F44" s="22">
         <f t="shared" si="7"/>
-        <v>7.6484122803781949</v>
+        <v>17.667924450993389</v>
       </c>
       <c r="G44" s="17">
         <f t="shared" si="8"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10278,19 +10281,19 @@
       </c>
       <c r="D45" s="22">
         <f t="shared" si="5"/>
-        <v>5.5370148247396225</v>
+        <v>9.9483448209912382</v>
       </c>
       <c r="E45" s="17">
         <f t="shared" si="6"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F45" s="22">
         <f t="shared" si="7"/>
-        <v>7.0813818391985546</v>
+        <v>16.358077305086137</v>
       </c>
       <c r="G45" s="17">
         <f t="shared" si="8"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10306,19 +10309,19 @@
       </c>
       <c r="D46" s="22">
         <f t="shared" si="5"/>
-        <v>5.126517084320346</v>
+        <v>9.2108042509927159</v>
       </c>
       <c r="E46" s="17">
         <f t="shared" si="6"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F46" s="22">
         <f t="shared" si="7"/>
-        <v>6.5563893412465903</v>
+        <v>15.145338314152067</v>
       </c>
       <c r="G46" s="17">
         <f t="shared" si="8"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10334,19 +10337,19 @@
       </c>
       <c r="D47" s="22">
         <f t="shared" si="5"/>
-        <v>4.7464524202469009</v>
+        <v>8.5279427358703277</v>
       </c>
       <c r="E47" s="17">
         <f t="shared" si="6"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F47" s="22">
         <f t="shared" si="7"/>
-        <v>6.0703182189758715</v>
+        <v>14.022508169636902</v>
       </c>
       <c r="G47" s="17">
         <f t="shared" si="8"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10362,19 +10365,19 @@
       </c>
       <c r="D48" s="22">
         <f t="shared" si="5"/>
-        <v>4.3945646151405482</v>
+        <v>7.8957065338181902</v>
       </c>
       <c r="E48" s="17">
         <f t="shared" si="6"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F48" s="22">
         <f t="shared" si="7"/>
-        <v>5.6202829578489082</v>
+        <v>12.982921298218784</v>
       </c>
       <c r="G48" s="17">
         <f t="shared" si="8"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10390,19 +10393,19 @@
       </c>
       <c r="D49" s="22">
         <f t="shared" si="5"/>
-        <v>4.0687647208398232</v>
+        <v>7.310342435339634</v>
       </c>
       <c r="E49" s="17">
         <f t="shared" si="6"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F49" s="22">
         <f t="shared" si="7"/>
-        <v>5.2036119667571601</v>
+        <v>12.020406292272279</v>
       </c>
       <c r="G49" s="17">
         <f t="shared" si="8"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10418,19 +10421,19 @@
       </c>
       <c r="D50" s="22">
         <f t="shared" si="5"/>
-        <v>3.767118657560415</v>
+        <v>6.7683754826795051</v>
       </c>
       <c r="E50" s="17">
         <f t="shared" si="6"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F50" s="22">
         <f t="shared" si="7"/>
-        <v>4.8178317183770254</v>
+        <v>11.129249273899747</v>
       </c>
       <c r="G50" s="17">
         <f t="shared" si="8"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10446,19 +10449,19 @@
       </c>
       <c r="D51" s="22">
         <f t="shared" si="5"/>
-        <v>3.487835732416257</v>
+        <v>6.2665883410711523</v>
       </c>
       <c r="E51" s="17">
         <f t="shared" si="6"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F51" s="22">
         <f t="shared" si="7"/>
-        <v>4.4606520653124173</v>
+        <v>10.304159975043921</v>
       </c>
       <c r="G51" s="17">
         <f t="shared" si="8"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10474,19 +10477,19 @@
       </c>
       <c r="D52" s="22">
         <f t="shared" si="5"/>
-        <v>3.2292580091431691</v>
+        <v>5.8020021993375517</v>
       </c>
       <c r="E52" s="17">
         <f t="shared" si="6"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F52" s="22">
         <f t="shared" si="7"/>
-        <v>4.1299526448546686</v>
+        <v>9.5402403323196054</v>
       </c>
       <c r="G52" s="17">
         <f t="shared" si="8"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10502,19 +10505,19 @@
       </c>
       <c r="D53" s="22">
         <f t="shared" si="5"/>
-        <v>2.9898504659194685</v>
+        <v>5.3718590864648608</v>
       </c>
       <c r="E53" s="17">
         <f t="shared" si="6"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F53" s="22">
         <f t="shared" si="7"/>
-        <v>3.8237702916529721</v>
+        <v>8.8329554101308307</v>
       </c>
       <c r="G53" s="17">
         <f t="shared" si="8"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10530,19 +10533,19 @@
       </c>
       <c r="D54" s="22">
         <f t="shared" si="5"/>
-        <v>2.7681918828563123</v>
+        <v>4.973605499172308</v>
       </c>
       <c r="E54" s="17">
         <f t="shared" si="6"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F54" s="22">
         <f t="shared" si="7"/>
-        <v>3.5402873835717701</v>
+        <v>8.1781064794611424</v>
       </c>
       <c r="G54" s="17">
         <f t="shared" si="8"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10558,19 +10561,19 @@
       </c>
       <c r="D55" s="22">
         <f t="shared" si="5"/>
-        <v>2.5629664050623386</v>
+        <v>4.6048772432852303</v>
       </c>
       <c r="E55" s="17">
         <f t="shared" si="6"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F55" s="22">
         <f t="shared" si="7"/>
-        <v>3.2778210515515314</v>
+        <v>7.5718060925220607</v>
       </c>
       <c r="G55" s="17">
         <f t="shared" si="8"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10586,19 +10589,19 @@
       </c>
       <c r="D56" s="22">
         <f t="shared" si="5"/>
-        <v>2.3729557311974583</v>
+        <v>4.2634853989233852</v>
       </c>
       <c r="E56" s="17">
         <f t="shared" si="6"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F56" s="22">
         <f t="shared" si="7"/>
-        <v>3.0348131894181813</v>
+        <v>7.0104550052926013</v>
       </c>
       <c r="G56" s="17">
         <f t="shared" si="8"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10614,19 +10617,19 @@
       </c>
       <c r="D57" s="22">
         <f t="shared" si="5"/>
-        <v>2.1970318811439506</v>
+        <v>3.9474033261882897</v>
       </c>
       <c r="E57" s="17">
         <f t="shared" si="6"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F57" s="22">
         <f t="shared" si="7"/>
-        <v>2.8098212043354285</v>
+        <v>6.4907208109527863</v>
       </c>
       <c r="G57" s="17">
         <f t="shared" si="8"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10642,19 +10645,19 @@
       </c>
       <c r="D58" s="22">
         <f t="shared" si="5"/>
-        <v>2.03415049986083</v>
+        <v>3.6547546342101116</v>
       </c>
       <c r="E58" s="17">
         <f t="shared" si="6"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F58" s="22">
         <f t="shared" si="7"/>
-        <v>2.6015094529909475</v>
+        <v>6.0095181573706205</v>
       </c>
       <c r="G58" s="17">
         <f t="shared" si="8"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10670,19 +10673,19 @@
       </c>
       <c r="D59" s="22">
         <f t="shared" si="5"/>
-        <v>1.8833446576704247</v>
+        <v>3.3838020421334432</v>
       </c>
       <c r="E59" s="17">
         <f t="shared" si="6"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F59" s="22">
         <f t="shared" si="7"/>
-        <v>2.4086413126781032</v>
+        <v>5.5639904312054158</v>
       </c>
       <c r="G59" s="17">
         <f t="shared" si="8"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10698,19 +10701,19 @@
       </c>
       <c r="D60" s="22">
         <f t="shared" si="5"/>
-        <v>1.7437191101732159</v>
+        <v>3.1329370659163636</v>
       </c>
       <c r="E60" s="17">
         <f t="shared" si="6"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F60" s="22">
         <f t="shared" si="7"/>
-        <v>2.2300718402040283</v>
+        <v>5.1514927998970652</v>
       </c>
       <c r="G60" s="17">
         <f t="shared" si="8"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10726,19 +10729,19 @@
       </c>
       <c r="D61" s="22">
         <f t="shared" si="5"/>
-        <v>1.6144449837154315</v>
+        <v>2.9006704697193877</v>
       </c>
       <c r="E61" s="17">
         <f t="shared" si="6"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F61" s="22">
         <f t="shared" si="7"/>
-        <v>2.0647409750443053</v>
+        <v>4.7695765108715324</v>
       </c>
       <c r="G61" s="17">
         <f t="shared" si="8"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10754,19 +10757,19 @@
       </c>
       <c r="D62" s="22">
         <f t="shared" si="5"/>
-        <v>1.4947548548601968</v>
+        <v>2.6856234251999176</v>
       </c>
       <c r="E62" s="17">
         <f t="shared" si="6"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F62" s="22">
         <f t="shared" si="7"/>
-        <v>1.9116672463954658</v>
+        <v>4.4159743547563517</v>
       </c>
       <c r="G62" s="17">
         <f t="shared" si="8"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10782,19 +10785,19 @@
       </c>
       <c r="D63" s="22">
         <f t="shared" si="5"/>
-        <v>1.3839381946520117</v>
+        <v>2.4865193262302197</v>
       </c>
       <c r="E63" s="17">
         <f t="shared" si="6"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F63" s="22">
         <f t="shared" si="7"/>
-        <v>1.7699419467678312</v>
+        <v>4.0885872063099509</v>
       </c>
       <c r="G63" s="17">
         <f t="shared" si="8"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10810,19 +10813,19 @@
       </c>
       <c r="D64" s="22">
         <f t="shared" si="5"/>
-        <v>1.2813371506298283</v>
+        <v>2.3021762104477217</v>
       </c>
       <c r="E64" s="17">
         <f t="shared" si="6"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F64" s="22">
         <f t="shared" si="7"/>
-        <v>1.6387237375307506</v>
+        <v>3.7854715631662019</v>
       </c>
       <c r="G64" s="17">
         <f t="shared" si="8"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10838,19 +10841,19 @@
       </c>
       <c r="D65" s="22">
         <f t="shared" si="5"/>
-        <v>1.1863426415491065</v>
+        <v>2.1314997426489843</v>
       </c>
       <c r="E65" s="17">
         <f t="shared" si="6"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F65" s="22">
         <f t="shared" si="7"/>
-        <v>1.5172336543866372</v>
+        <v>3.5048280084193122</v>
       </c>
       <c r="G65" s="17">
         <f t="shared" si="8"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10866,19 +10869,19 @@
       </c>
       <c r="D66" s="22">
         <f t="shared" si="5"/>
-        <v>1.0983907416294878</v>
+        <v>1.9734767183738373</v>
       </c>
       <c r="E66" s="17">
         <f t="shared" si="6"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F66" s="22">
         <f t="shared" si="7"/>
-        <v>1.4047504831242079</v>
+        <v>3.2449905285581346</v>
       </c>
       <c r="G66" s="17">
         <f t="shared" si="8"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10894,19 +10897,19 @@
       </c>
       <c r="D67" s="22">
         <f t="shared" ref="D67:D94" si="10">IF($B67&lt;$K$10/$A67,$B67,$K$10/$A67)</f>
-        <v>1.0169593328635618</v>
+        <v>1.8271690491144155</v>
       </c>
       <c r="E67" s="17">
         <f t="shared" ref="E67:E94" si="11">IF($D67=$B67,$C67,$K$10)</f>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F67" s="22">
         <f t="shared" ref="F67:F94" si="12">IF($B67&lt;$K$11/$A67,$B67,$K$11/$A67)</f>
-        <v>1.300606478199587</v>
+        <v>3.0044166233369713</v>
       </c>
       <c r="G67" s="17">
         <f t="shared" ref="G67:G94" si="13">IF($D67=$B67,$C67,$K$11)</f>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10922,19 +10925,19 @@
       </c>
       <c r="D68" s="22">
         <f t="shared" si="10"/>
-        <v>0.94156500551345956</v>
+        <v>1.6917081934428257</v>
       </c>
       <c r="E68" s="17">
         <f t="shared" si="11"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F68" s="22">
         <f t="shared" si="12"/>
-        <v>1.2041833987290149</v>
+        <v>2.7816781488710052</v>
       </c>
       <c r="G68" s="17">
         <f t="shared" si="13"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10950,19 +10953,19 @@
       </c>
       <c r="D69" s="22">
         <f t="shared" si="10"/>
-        <v>0.8777965868394163</v>
+        <v>1.5771355874920097</v>
       </c>
       <c r="E69" s="17">
         <f t="shared" si="11"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F69" s="22">
         <f t="shared" si="12"/>
-        <v>1.1226288903511155</v>
+        <v>2.5932862526397806</v>
       </c>
       <c r="G69" s="17">
         <f t="shared" si="13"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10978,19 +10981,19 @@
       </c>
       <c r="D70" s="22">
         <f t="shared" si="10"/>
-        <v>0.81493958561453539</v>
+        <v>1.464200523673034</v>
       </c>
       <c r="E70" s="17">
         <f t="shared" si="11"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F70" s="22">
         <f t="shared" si="12"/>
-        <v>1.0422400091526107</v>
+        <v>2.4075869692265659</v>
       </c>
       <c r="G70" s="17">
         <f t="shared" si="13"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11006,19 +11009,19 @@
       </c>
       <c r="D71" s="22">
         <f t="shared" si="10"/>
-        <v>0.75452239890622275</v>
+        <v>1.3556490703153545</v>
       </c>
       <c r="E71" s="17">
         <f t="shared" si="11"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F71" s="22">
         <f t="shared" si="12"/>
-        <v>0.96497144797410017</v>
+        <v>2.2290956626267362</v>
       </c>
       <c r="G71" s="17">
         <f t="shared" si="13"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11034,19 +11037,19 @@
       </c>
       <c r="D72" s="22">
         <f t="shared" si="10"/>
-        <v>0.69858436195843443</v>
+        <v>1.2551452974738009</v>
       </c>
       <c r="E72" s="17">
         <f t="shared" si="11"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F72" s="22">
         <f t="shared" si="12"/>
-        <v>0.89343134712542449</v>
+        <v>2.0638371683568182</v>
       </c>
       <c r="G72" s="17">
         <f t="shared" si="13"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11062,19 +11065,19 @@
       </c>
       <c r="D73" s="22">
         <f t="shared" si="10"/>
-        <v>0.64679340398684038</v>
+        <v>1.1620925741527808</v>
       </c>
       <c r="E73" s="17">
         <f t="shared" si="11"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F73" s="22">
         <f t="shared" si="12"/>
-        <v>0.82719501566825004</v>
+        <v>1.91083044523618</v>
       </c>
       <c r="G73" s="17">
         <f t="shared" si="13"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11090,19 +11093,19 @@
       </c>
       <c r="D74" s="22">
         <f t="shared" si="10"/>
-        <v>0.5988420729431897</v>
+        <v>1.0759385017966225</v>
       </c>
       <c r="E74" s="17">
         <f t="shared" si="11"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F74" s="22">
         <f t="shared" si="12"/>
-        <v>0.76586924798189138</v>
+        <v>1.769167183547026</v>
       </c>
       <c r="G74" s="17">
         <f t="shared" si="13"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11118,19 +11121,19 @@
       </c>
       <c r="D75" s="22">
         <f t="shared" si="10"/>
-        <v>0.55444571035574841</v>
+        <v>0.99617163502859096</v>
       </c>
       <c r="E75" s="17">
         <f t="shared" si="11"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F75" s="22">
         <f t="shared" si="12"/>
-        <v>0.7090899895358993</v>
+        <v>1.6380064129409713</v>
       </c>
       <c r="G75" s="17">
         <f t="shared" si="13"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11146,19 +11149,19 @@
       </c>
       <c r="D76" s="22">
         <f t="shared" si="10"/>
-        <v>0.51334076148162311</v>
+        <v>0.92231844550453301</v>
       </c>
       <c r="E76" s="17">
         <f t="shared" si="11"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F76" s="22">
         <f t="shared" si="12"/>
-        <v>0.65652017571530796</v>
+        <v>1.5165695100993439</v>
       </c>
       <c r="G76" s="17">
         <f t="shared" si="13"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11174,19 +11177,19 @@
       </c>
       <c r="D77" s="22">
         <f t="shared" si="10"/>
-        <v>0.47528321073933727</v>
+        <v>0.85394051085733169</v>
       </c>
       <c r="E77" s="17">
         <f t="shared" si="11"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F77" s="22">
         <f t="shared" si="12"/>
-        <v>0.60784773086891486</v>
+        <v>1.4041355765106209</v>
       </c>
       <c r="G77" s="17">
         <f t="shared" si="13"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11202,19 +11205,19 @@
       </c>
       <c r="D78" s="22">
         <f t="shared" si="10"/>
-        <v>0.44004713313376675</v>
+        <v>0.79063191204463001</v>
       </c>
       <c r="E78" s="17">
         <f t="shared" si="11"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F78" s="22">
         <f t="shared" si="12"/>
-        <v>0.56278371570214825</v>
+        <v>1.300037158925647</v>
       </c>
       <c r="G78" s="17">
         <f t="shared" si="13"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11230,19 +11233,19 @@
       </c>
       <c r="D79" s="22">
         <f t="shared" si="10"/>
-        <v>0.40742335307410504</v>
+        <v>0.73201682364942156</v>
       </c>
       <c r="E79" s="17">
         <f t="shared" si="11"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F79" s="22">
         <f t="shared" si="12"/>
-        <v>0.52106061201669618</v>
+        <v>1.203656287085527</v>
       </c>
       <c r="G79" s="17">
         <f t="shared" si="13"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11258,19 +11261,19 @@
       </c>
       <c r="D80" s="22">
         <f t="shared" si="10"/>
-        <v>0.37721820262305267</v>
+        <v>0.67774728282854824</v>
       </c>
       <c r="E80" s="17">
         <f t="shared" si="11"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F80" s="22">
         <f t="shared" si="12"/>
-        <v>0.48243073461440833</v>
+        <v>1.1144208052005193</v>
       </c>
       <c r="G80" s="17">
         <f t="shared" si="13"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11286,19 +11289,19 @@
       </c>
       <c r="D81" s="22">
         <f t="shared" si="10"/>
-        <v>0.34925237180571045</v>
+        <v>0.62750112366470556</v>
       </c>
       <c r="E81" s="17">
         <f t="shared" si="11"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F81" s="22">
         <f t="shared" si="12"/>
-        <v>0.44666476093790852</v>
+        <v>1.0318009754021482</v>
       </c>
       <c r="G81" s="17">
         <f t="shared" si="13"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11314,19 +11317,19 @@
       </c>
       <c r="D82" s="22">
         <f t="shared" si="10"/>
-        <v>0.32335984415312985</v>
+        <v>0.58098006465940732</v>
       </c>
       <c r="E82" s="17">
         <f t="shared" si="11"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F82" s="22">
         <f t="shared" si="12"/>
-        <v>0.41355036971925169</v>
+        <v>0.95530633300521173</v>
       </c>
       <c r="G82" s="17">
         <f t="shared" si="13"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11342,19 +11345,19 @@
       </c>
       <c r="D83" s="22">
         <f t="shared" si="10"/>
-        <v>0.29794903266040068</v>
+        <v>0.53532450423334965</v>
       </c>
       <c r="E83" s="17">
         <f t="shared" si="11"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F83" s="22">
         <f t="shared" si="12"/>
-        <v>0.38105205343880499</v>
+        <v>0.86429450919459005</v>
       </c>
       <c r="G83" s="17">
         <f t="shared" si="13"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11370,19 +11373,19 @@
       </c>
       <c r="D84" s="22">
         <f t="shared" si="10"/>
-        <v>0.27719125981633252</v>
+        <v>0.49802905018364718</v>
       </c>
       <c r="E84" s="17">
         <f t="shared" si="11"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F84" s="22">
         <f t="shared" si="12"/>
-        <v>0.35450458692608788</v>
+        <v>0.76337281522955247</v>
       </c>
       <c r="G84" s="17">
         <f t="shared" si="13"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11398,19 +11401,19 @@
       </c>
       <c r="D85" s="22">
         <f t="shared" si="10"/>
-        <v>0.25664112776500114</v>
+        <v>0.46110666398195194</v>
       </c>
       <c r="E85" s="17">
         <f t="shared" si="11"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F85" s="22">
         <f t="shared" si="12"/>
-        <v>0.32822267573249214</v>
+        <v>0.6794182695875215</v>
       </c>
       <c r="G85" s="17">
         <f t="shared" si="13"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11426,19 +11429,19 @@
       </c>
       <c r="D86" s="22">
         <f t="shared" si="10"/>
-        <v>0.23761452112210815</v>
+        <v>0.42692159320859291</v>
       </c>
       <c r="E86" s="17">
         <f t="shared" si="11"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F86" s="22">
         <f t="shared" si="12"/>
-        <v>0.30388922693250758</v>
+        <v>0.60469691327754749</v>
       </c>
       <c r="G86" s="17">
         <f t="shared" si="13"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11454,19 +11457,19 @@
       </c>
       <c r="D87" s="22">
         <f t="shared" si="10"/>
-        <v>0.21999849026453824</v>
+        <v>0.39527090147388755</v>
       </c>
       <c r="E87" s="17">
         <f t="shared" si="11"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F87" s="22">
         <f t="shared" si="12"/>
-        <v>0.28135978734419603</v>
+        <v>0.53840446288357602</v>
       </c>
       <c r="G87" s="17">
         <f t="shared" si="13"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="88" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11482,19 +11485,19 @@
       </c>
       <c r="D88" s="22">
         <f t="shared" si="10"/>
-        <v>0.203688459316862</v>
+        <v>0.36596669748592875</v>
       </c>
       <c r="E88" s="17">
         <f t="shared" si="11"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F88" s="22">
         <f t="shared" si="12"/>
-        <v>0.26050061311305744</v>
+        <v>0.47900363967956822</v>
       </c>
       <c r="G88" s="17">
         <f t="shared" si="13"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="89" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11510,19 +11513,19 @@
       </c>
       <c r="D89" s="22">
         <f t="shared" si="10"/>
-        <v>0.18858760534669269</v>
+        <v>0.33883501965197188</v>
       </c>
       <c r="E89" s="17">
         <f t="shared" si="11"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F89" s="22">
         <f t="shared" si="12"/>
-        <v>0.24118787575447997</v>
+        <v>0.42632357021955675</v>
       </c>
       <c r="G89" s="17">
         <f t="shared" si="13"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11538,19 +11541,19 @@
       </c>
       <c r="D90" s="22">
         <f t="shared" si="10"/>
-        <v>0.17460628358464719</v>
+        <v>0.31371480337214674</v>
       </c>
       <c r="E90" s="17">
         <f t="shared" si="11"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F90" s="22">
         <f t="shared" si="12"/>
-        <v>0.22330692705783342</v>
+        <v>0.37958605013304503</v>
       </c>
       <c r="G90" s="17">
         <f t="shared" si="13"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="91" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11566,19 +11569,19 @@
       </c>
       <c r="D91" s="22">
         <f t="shared" si="10"/>
-        <v>0.16166149525678214</v>
+        <v>0.29045692489492958</v>
       </c>
       <c r="E91" s="17">
         <f t="shared" si="11"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F91" s="22">
         <f t="shared" si="12"/>
-        <v>0.20675161848837811</v>
+        <v>0.33923104342632693</v>
       </c>
       <c r="G91" s="17">
         <f t="shared" si="13"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="92" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11594,19 +11597,19 @@
       </c>
       <c r="D92" s="22">
         <f t="shared" si="10"/>
-        <v>0.14967639487034218</v>
+        <v>0.26892331605831116</v>
       </c>
       <c r="E92" s="17">
         <f t="shared" si="11"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F92" s="22">
         <f t="shared" si="12"/>
-        <v>0.19142367104668084</v>
+        <v>0.31125786554921364</v>
       </c>
       <c r="G92" s="17">
         <f t="shared" si="13"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11622,19 +11625,19 @@
       </c>
       <c r="D93" s="22">
         <f t="shared" si="10"/>
-        <v>0.14025782871073497</v>
+        <v>0.25200099476409327</v>
       </c>
       <c r="E93" s="17">
         <f t="shared" si="11"/>
-        <v>90.56825948592487</v>
+        <v>162.72383291756145</v>
       </c>
       <c r="F93" s="22">
         <f t="shared" si="12"/>
-        <v>0.17937810760409625</v>
+        <v>0.28067652277033595</v>
       </c>
       <c r="G93" s="17">
         <f t="shared" si="13"/>
-        <v>115.82927773028129</v>
+        <v>267.56702608747815</v>
       </c>
     </row>
     <row r="94" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -11650,19 +11653,19 @@
       </c>
       <c r="D94" s="23">
         <f t="shared" si="10"/>
-        <v>0.13791427064949893</v>
+        <v>0.22422064894203664</v>
       </c>
       <c r="E94" s="21">
         <f t="shared" si="11"/>
-        <v>90.56825948592487</v>
+        <v>147.24563179610752</v>
       </c>
       <c r="F94" s="23">
         <f t="shared" si="12"/>
-        <v>0.17638089159163514</v>
+        <v>0.22422064894203664</v>
       </c>
       <c r="G94" s="21">
         <f t="shared" si="13"/>
-        <v>115.82927773028129</v>
+        <v>147.24563179610752</v>
       </c>
     </row>
     <row r="95" spans="1:7" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Simulation, layout & info - V4A
</commit_message>
<xml_diff>
--- a/DOCS/MOSFET comparison.xlsx
+++ b/DOCS/MOSFET comparison.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA4BAF71-8113-4913-8BCA-8BBA3847C4DF}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F76830-C494-4BF4-BAB7-C6000353E8F3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="594" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,10 +20,16 @@
     <definedName name="tA">Comparison!$B$38</definedName>
     <definedName name="tJmax">Comparison!$B$39</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -2974,7 +2980,7 @@
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent3">
-                  <a:shade val="76000"/>
+                  <a:shade val="65000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -3315,241 +3321,241 @@
                   <c:v>46.92853011606438</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="0.0">
-                  <c:v>50.354147410673434</c:v>
+                  <c:v>45.682726020188127</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="0.0">
-                  <c:v>51.823341619826913</c:v>
+                  <c:v>42.33883278672841</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="0.0">
-                  <c:v>48.288696073878597</c:v>
+                  <c:v>39.451084485430044</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="0.0">
-                  <c:v>45.205429625153542</c:v>
+                  <c:v>36.932105613570563</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="0.0">
-                  <c:v>42.492269028999353</c:v>
+                  <c:v>34.715497243411662</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="0.0">
-                  <c:v>40.110611454437382</c:v>
+                  <c:v>32.769721485754893</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="0.0">
-                  <c:v>37.938274821439656</c:v>
+                  <c:v>30.994957555329627</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="0.0">
-                  <c:v>36.008706853213063</c:v>
+                  <c:v>29.418531701576548</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0.0">
-                  <c:v>34.265917616088096</c:v>
+                  <c:v>27.994701053324526</c:v>
                 </c:pt>
                 <c:pt idx="22" formatCode="0.0">
-                  <c:v>32.68403931704993</c:v>
+                  <c:v>26.702332041629852</c:v>
                 </c:pt>
                 <c:pt idx="23" formatCode="0.0">
-                  <c:v>31.241770100751051</c:v>
+                  <c:v>25.524021394850529</c:v>
                 </c:pt>
                 <c:pt idx="24" formatCode="0.0">
-                  <c:v>29.921409205725816</c:v>
+                  <c:v>24.445307876862703</c:v>
                 </c:pt>
                 <c:pt idx="25" formatCode="0.0">
-                  <c:v>28.708126861139302</c:v>
+                  <c:v>23.454075804500832</c:v>
                 </c:pt>
                 <c:pt idx="26" formatCode="0.0">
-                  <c:v>27.589404891130879</c:v>
+                  <c:v>22.540098030344627</c:v>
                 </c:pt>
                 <c:pt idx="27" formatCode="0.0">
-                  <c:v>26.554603207389672</c:v>
+                  <c:v>21.694681774157434</c:v>
                 </c:pt>
                 <c:pt idx="28" formatCode="0.0">
-                  <c:v>25.59462033281774</c:v>
+                  <c:v>20.91039127620402</c:v>
                 </c:pt>
                 <c:pt idx="29" formatCode="0.0">
-                  <c:v>24.701624991093023</c:v>
+                  <c:v>20.180828510260245</c:v>
                 </c:pt>
                 <c:pt idx="30" formatCode="0.0">
-                  <c:v>23.868841990874635</c:v>
+                  <c:v>19.500458254468274</c:v>
                 </c:pt>
                 <c:pt idx="31" formatCode="0.0">
-                  <c:v>23.090380009235478</c:v>
+                  <c:v>18.86446739318356</c:v>
                 </c:pt>
                 <c:pt idx="32" formatCode="0.0">
-                  <c:v>22.361092010887415</c:v>
+                  <c:v>18.268650881737042</c:v>
                 </c:pt>
                 <c:pt idx="33" formatCode="0.0">
-                  <c:v>21.676461308717052</c:v>
+                  <c:v>17.709318659733785</c:v>
                 </c:pt>
                 <c:pt idx="34" formatCode="0.0">
-                  <c:v>21.032507933458092</c:v>
+                  <c:v>17.183219156588134</c:v>
                 </c:pt>
                 <c:pt idx="35" formatCode="0.0">
-                  <c:v>20.516775460725057</c:v>
+                  <c:v>16.761874059123869</c:v>
                 </c:pt>
                 <c:pt idx="36" formatCode="0.0">
-                  <c:v>15.826792866650564</c:v>
+                  <c:v>12.93023405644181</c:v>
                 </c:pt>
                 <c:pt idx="37" formatCode="0.0">
-                  <c:v>14.622351394453444</c:v>
+                  <c:v>11.946224833978917</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>13.538293938038368</c:v>
+                  <c:v>11.060567407349287</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>12.534605263435964</c:v>
+                  <c:v>10.240569976931441</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>11.605327069218733</c:v>
+                  <c:v>9.4813647067281881</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>10.744942784629968</c:v>
+                  <c:v>8.7784446475632656</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>9.9483448209912382</c:v>
+                  <c:v>8.1276369820103938</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>9.2108042509927159</c:v>
+                  <c:v>7.5250782528633549</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>8.5279427358703277</c:v>
+                  <c:v>6.9671914280933036</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>7.8957065338181902</c:v>
+                  <c:v>6.4506646661416864</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>7.310342435339634</c:v>
+                  <c:v>5.9724316554908308</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>6.7683754826795051</c:v>
+                  <c:v>5.5296534118001341</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>6.2665883410711523</c:v>
+                  <c:v>5.1197014245481505</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>5.8020021993375517</c:v>
+                  <c:v>4.7401420531323035</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>5.3718590864648608</c:v>
+                  <c:v>4.3887220797951896</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>4.973605499172308</c:v>
+                  <c:v>4.0633553336137131</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>4.6048772432852303</c:v>
+                  <c:v>3.7621103061457775</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>4.2634853989233852</c:v>
+                  <c:v>3.4831986852158949</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>3.9474033261882897</c:v>
+                  <c:v>3.2249647387716975</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>3.6547546342101116</c:v>
+                  <c:v>2.9858754857896308</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>3.3838020421334432</c:v>
+                  <c:v>2.7645115958803061</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>3.1329370659163636</c:v>
+                  <c:v>2.559558963569966</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>2.9006704697193877</c:v>
+                  <c:v>2.3698009072395338</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>2.6856234251999176</c:v>
+                  <c:v>2.1941109464110218</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>2.4865193262302197</c:v>
+                  <c:v>2.0314461145043676</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>2.3021762104477217</c:v>
+                  <c:v>1.8808407673664738</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>2.1314997426489843</c:v>
+                  <c:v>1.7414008508174508</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>1.9734767183738373</c:v>
+                  <c:v>1.6122985931838196</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>1.8271690491144155</c:v>
+                  <c:v>1.4927675913114762</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>1.6917081934428257</c:v>
+                  <c:v>1.3820982608869719</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>1.5771355874920097</c:v>
+                  <c:v>1.2884942929900918</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>1.464200523673034</c:v>
+                  <c:v>1.1962281705569378</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>1.3556490703153545</c:v>
+                  <c:v>1.1075433870440816</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>1.2551452974738009</c:v>
+                  <c:v>1.0254334284854485</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>1.1620925741527808</c:v>
+                  <c:v>0.94941085699748629</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>1.0759385017966225</c:v>
+                  <c:v>0.87902437188538896</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.99617163502859096</c:v>
+                  <c:v>0.81385613053985506</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.92231844550453301</c:v>
+                  <c:v>0.75351926795457247</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.85394051085733169</c:v>
+                  <c:v>0.69765560013925554</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.79063191204463001</c:v>
+                  <c:v>0.64593349779478693</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>0.73201682364942156</c:v>
+                  <c:v>0.59804591762773385</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.67774728282854824</c:v>
+                  <c:v>0.55370857961731856</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>0.62750112366470556</c:v>
+                  <c:v>0.51265827941438114</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.58098006465940732</c:v>
+                  <c:v>0.47465132585403252</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.53532450423334965</c:v>
+                  <c:v>0.43735147064894686</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.49802905018364718</c:v>
+                  <c:v>0.40688168727798524</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.46110666398195194</c:v>
+                  <c:v>0.3767166943111383</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.42692159320859291</c:v>
+                  <c:v>0.34878804382207018</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>0.39527090147388755</c:v>
+                  <c:v>0.32292994005928061</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>0.36596669748592875</c:v>
+                  <c:v>0.29898887887306619</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>0.33883501965197188</c:v>
+                  <c:v>0.27682273645287536</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>0.31371480337214674</c:v>
+                  <c:v>0.2562999256229565</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>0.29045692489492958</c:v>
+                  <c:v>0.23729861468772706</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>0.26892331605831116</c:v>
+                  <c:v>0.21970600418961136</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>0.25200099476409327</c:v>
+                  <c:v>0.20588074110844654</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>0.22422064894203664</c:v>
+                  <c:v>0.20244069448207935</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3578,8 +3584,611 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>IXTK102N65X2!$A$3:$A$94</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="92"/>
+                <c:pt idx="0">
+                  <c:v>2.8288034520991268E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25370830961014068</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.43492853076024085</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.66476881124329523</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.88576908093853923</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.1067693506337837</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.3366096311168381</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.566449911599892</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.7962901920829464</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.0084504509903804</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.2206107098978154</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.4504509903808693</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.6802912708639233</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.9101315513469781</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.139971831830032</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.369812112313086</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.5996523927961399</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.8294926732791947</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.0568773952100781</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.2891732342453022</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4.519013514728357</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4.74885379521141</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4.9786940756944649</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5.2085343561775197</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5.4383746366605727</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5.6682149171436276</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>5.8980551976266806</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>6.1278954781097354</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>6.3577357585927903</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>6.5875760390758433</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>6.8174163195588982</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>7.0472566000419512</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>7.277096880525006</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>7.5069371610080609</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>7.7367774414911139</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>7.931257678822929</c:v>
+                </c:pt>
+                <c:pt idx="36" formatCode="0.0">
+                  <c:v>10.281541831538409</c:v>
+                </c:pt>
+                <c:pt idx="37" formatCode="0.0">
+                  <c:v>11.128431298627245</c:v>
+                </c:pt>
+                <c:pt idx="38" formatCode="0.0">
+                  <c:v>12.019522818924651</c:v>
+                </c:pt>
+                <c:pt idx="39" formatCode="0.0">
+                  <c:v>12.981967082141356</c:v>
+                </c:pt>
+                <c:pt idx="40" formatCode="0.0">
+                  <c:v>14.021477546217572</c:v>
+                </c:pt>
+                <c:pt idx="41" formatCode="0.0">
+                  <c:v>15.14422516519387</c:v>
+                </c:pt>
+                <c:pt idx="42" formatCode="0.0">
+                  <c:v>16.356875022487198</c:v>
+                </c:pt>
+                <c:pt idx="43" formatCode="0.0">
+                  <c:v>17.666625897518504</c:v>
+                </c:pt>
+                <c:pt idx="44" formatCode="0.0">
+                  <c:v>19.081253000575469</c:v>
+                </c:pt>
+                <c:pt idx="45" formatCode="0.0">
+                  <c:v>20.609154129601595</c:v>
+                </c:pt>
+                <c:pt idx="46" formatCode="0.0">
+                  <c:v>22.259399522917342</c:v>
+                </c:pt>
+                <c:pt idx="47" formatCode="0.0">
+                  <c:v>24.04178570381875</c:v>
+                </c:pt>
+                <c:pt idx="48" formatCode="0.0">
+                  <c:v>25.966893636697215</c:v>
+                </c:pt>
+                <c:pt idx="49" formatCode="0.0">
+                  <c:v>28.046151539918508</c:v>
+                </c:pt>
+                <c:pt idx="50" formatCode="0.0">
+                  <c:v>30.291902728343448</c:v>
+                </c:pt>
+                <c:pt idx="51" formatCode="0.0">
+                  <c:v>32.717478888231376</c:v>
+                </c:pt>
+                <c:pt idx="52" formatCode="0.0">
+                  <c:v>35.337279219515167</c:v>
+                </c:pt>
+                <c:pt idx="53" formatCode="0.0">
+                  <c:v>38.166855915268869</c:v>
+                </c:pt>
+                <c:pt idx="54" formatCode="0.0">
+                  <c:v>41.223006485808384</c:v>
+                </c:pt>
+                <c:pt idx="55" formatCode="0.0">
+                  <c:v>44.523873475498128</c:v>
+                </c:pt>
+                <c:pt idx="56" formatCode="0.0">
+                  <c:v>48.089052164223588</c:v>
+                </c:pt>
+                <c:pt idx="57" formatCode="0.0">
+                  <c:v>51.939706892888317</c:v>
+                </c:pt>
+                <c:pt idx="58" formatCode="0.0">
+                  <c:v>56.098696703491257</c:v>
+                </c:pt>
+                <c:pt idx="59" formatCode="0.0">
+                  <c:v>60.590711039634421</c:v>
+                </c:pt>
+                <c:pt idx="60" formatCode="0.0">
+                  <c:v>65.442416313033448</c:v>
+                </c:pt>
+                <c:pt idx="61" formatCode="0.0">
+                  <c:v>70.682614206110358</c:v>
+                </c:pt>
+                <c:pt idx="62" formatCode="0.0">
+                  <c:v>76.342412650414673</c:v>
+                </c:pt>
+                <c:pt idx="63" formatCode="0.0">
+                  <c:v>82.455410495872158</c:v>
+                </c:pt>
+                <c:pt idx="64" formatCode="0.0">
+                  <c:v>89.057896967130517</c:v>
+                </c:pt>
+                <c:pt idx="65" formatCode="0.0">
+                  <c:v>96.189067091056202</c:v>
+                </c:pt>
+                <c:pt idx="66" formatCode="0.0">
+                  <c:v>103.17681891658276</c:v>
+                </c:pt>
+                <c:pt idx="67" formatCode="0.0">
+                  <c:v>111.13493697527102</c:v>
+                </c:pt>
+                <c:pt idx="68" formatCode="0.0">
+                  <c:v>120.03389113062146</c:v>
+                </c:pt>
+                <c:pt idx="69" formatCode="0.0">
+                  <c:v>129.64541495321026</c:v>
+                </c:pt>
+                <c:pt idx="70" formatCode="0.0">
+                  <c:v>140.02656633116743</c:v>
+                </c:pt>
+                <c:pt idx="71" formatCode="0.0">
+                  <c:v>151.23897197269372</c:v>
+                </c:pt>
+                <c:pt idx="72" formatCode="0.0">
+                  <c:v>163.34919324709657</c:v>
+                </c:pt>
+                <c:pt idx="73" formatCode="0.0">
+                  <c:v>176.42912131996573</c:v>
+                </c:pt>
+                <c:pt idx="74" formatCode="0.0">
+                  <c:v>190.55640392817457</c:v>
+                </c:pt>
+                <c:pt idx="75" formatCode="0.0">
+                  <c:v>205.81490632821297</c:v>
+                </c:pt>
+                <c:pt idx="76" formatCode="0.0">
+                  <c:v>222.29520915422754</c:v>
+                </c:pt>
+                <c:pt idx="77" formatCode="0.0">
+                  <c:v>240.09514614125897</c:v>
+                </c:pt>
+                <c:pt idx="78" formatCode="0.0">
+                  <c:v>259.32038490581277</c:v>
+                </c:pt>
+                <c:pt idx="79" formatCode="0.0">
+                  <c:v>280.08505423151888</c:v>
+                </c:pt>
+                <c:pt idx="80" formatCode="0.0">
+                  <c:v>303.97232263933432</c:v>
+                </c:pt>
+                <c:pt idx="81" formatCode="0.0">
+                  <c:v>326.73562487480876</c:v>
+                </c:pt>
+                <c:pt idx="82" formatCode="0.0">
+                  <c:v>352.89846282492806</c:v>
+                </c:pt>
+                <c:pt idx="83" formatCode="0.0">
+                  <c:v>381.15624860899214</c:v>
+                </c:pt>
+                <c:pt idx="84" formatCode="0.0">
+                  <c:v>411.67673185857154</c:v>
+                </c:pt>
+                <c:pt idx="85" formatCode="0.0">
+                  <c:v>444.64109449144098</c:v>
+                </c:pt>
+                <c:pt idx="86" formatCode="0.0">
+                  <c:v>480.24502628063721</c:v>
+                </c:pt>
+                <c:pt idx="87" formatCode="0.0">
+                  <c:v>518.69988654800261</c:v>
+                </c:pt>
+                <c:pt idx="88" formatCode="0.0">
+                  <c:v>560.23395887849972</c:v>
+                </c:pt>
+                <c:pt idx="89" formatCode="0.0">
+                  <c:v>605.09380630379303</c:v>
+                </c:pt>
+                <c:pt idx="90" formatCode="0.0">
+                  <c:v>645.72694671262229</c:v>
+                </c:pt>
+                <c:pt idx="91" formatCode="0.0">
+                  <c:v>656.69969510333567</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>IXTK102N65X2!$F$3:$F$94</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="92"/>
+                <c:pt idx="0">
+                  <c:v>0.82764101964858128</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.6534462395073035</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.4909450910800359</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.0">
+                  <c:v>12.583047120130047</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.0">
+                  <c:v>16.47116797429733</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.0">
+                  <c:v>20.326083377421938</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.0">
+                  <c:v>24.166272143329934</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.0">
+                  <c:v>28.019478024333566</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.0">
+                  <c:v>31.766421754415916</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.0">
+                  <c:v>35.87707897479271</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="0.0">
+                  <c:v>39.466477977598117</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="0.0">
+                  <c:v>43.269076398215475</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="0.0">
+                  <c:v>46.92853011606438</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="0.0">
+                  <c:v>50.354147410673434</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="0.0">
+                  <c:v>53.89215007900944</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="0.0">
+                  <c:v>57.280946563595151</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="0.0">
+                  <c:v>54.321995436930095</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="0.0">
+                  <c:v>51.061672534436589</c:v>
+                </c:pt>
+                <c:pt idx="18" formatCode="0.0">
+                  <c:v>48.199706771242148</c:v>
+                </c:pt>
+                <c:pt idx="19" formatCode="0.0">
+                  <c:v>45.589275642864663</c:v>
+                </c:pt>
+                <c:pt idx="20" formatCode="0.0">
+                  <c:v>43.270572265097677</c:v>
+                </c:pt>
+                <c:pt idx="21" formatCode="0.0">
+                  <c:v>41.176315230673744</c:v>
+                </c:pt>
+                <c:pt idx="22" formatCode="0.0">
+                  <c:v>39.27541999630315</c:v>
+                </c:pt>
+                <c:pt idx="23" formatCode="0.0">
+                  <c:v>37.542288767681484</c:v>
+                </c:pt>
+                <c:pt idx="24" formatCode="0.0">
+                  <c:v>35.955651075939429</c:v>
+                </c:pt>
+                <c:pt idx="25" formatCode="0.0">
+                  <c:v>34.497686434681739</c:v>
+                </c:pt>
+                <c:pt idx="26" formatCode="0.0">
+                  <c:v>33.153352131171964</c:v>
+                </c:pt>
+                <c:pt idx="27" formatCode="0.0">
+                  <c:v>31.909862293591942</c:v>
+                </c:pt>
+                <c:pt idx="28" formatCode="0.0">
+                  <c:v>30.756279952611141</c:v>
+                </c:pt>
+                <c:pt idx="29" formatCode="0.0">
+                  <c:v>29.683194500695027</c:v>
+                </c:pt>
+                <c:pt idx="30" formatCode="0.0">
+                  <c:v>28.682464395640473</c:v>
+                </c:pt>
+                <c:pt idx="31" formatCode="0.0">
+                  <c:v>27.747010213143422</c:v>
+                </c:pt>
+                <c:pt idx="32" formatCode="0.0">
+                  <c:v>26.870646916809928</c:v>
+                </c:pt>
+                <c:pt idx="33" formatCode="0.0">
+                  <c:v>26.047946940553381</c:v>
+                </c:pt>
+                <c:pt idx="34" formatCode="0.0">
+                  <c:v>25.274127675866012</c:v>
+                </c:pt>
+                <c:pt idx="35" formatCode="0.0">
+                  <c:v>24.65438758573109</c:v>
+                </c:pt>
+                <c:pt idx="36" formatCode="0.0">
+                  <c:v>19.018577569386601</c:v>
+                </c:pt>
+                <c:pt idx="37" formatCode="0.0">
+                  <c:v>17.571236736675313</c:v>
+                </c:pt>
+                <c:pt idx="38" formatCode="0.0">
+                  <c:v>16.268557729107982</c:v>
+                </c:pt>
+                <c:pt idx="39" formatCode="0.0">
+                  <c:v>15.062455452148036</c:v>
+                </c:pt>
+                <c:pt idx="40" formatCode="0.0">
+                  <c:v>13.945769995456384</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>12.911872263060292</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>11.954624620361798</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>11.068344458659334</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>10.247770460886878</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>9.4880313683105282</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>8.7846170627687563</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>8.133351792789135</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>7.5303693846407116</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>6.9720902911649381</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>6.4552003421377613</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>5.976631070016313</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>5.5335414942760623</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>5.1233012562027511</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>4.7434750040204854</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>4.391807935659819</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>4.0662124133417814</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>3.7647555705167091</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>3.485647837587591</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>3.2272323183020073</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>2.9879749537466695</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>2.7664554155539762</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2.5613586742590888</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>2.3714671927537787</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>2.1956536984943225</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>2.0328744915563073</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1.8951960615697838</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1.7594854163593641</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1.6290424230538234</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>1.5082700836476013</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1.396451444746186</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>1.2929227057382493</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>1.1970692782070538</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>1.1083221374853491</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>1.0261544446950752</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.95007841921895764</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.87964244303772343</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.8144283797430919</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.75404909231115091</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.6981461449005858</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.64328324091537969</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.59846642352185853</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.55409791046047541</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.51301874643173118</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.47498506892340669</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.43977109466154035</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.40716777926970132</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.37698157629712592</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.33923104342632693</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.31125786554921364</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.28067652277033595</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.22422064894203664</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-3663-4392-BE33-75603037D070}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>IXTK102N65X2!#REF!</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>#REF!</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
                 <a:schemeClr val="accent3">
-                  <a:tint val="77000"/>
+                  <a:tint val="65000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -3876,285 +4485,12 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>IXTK102N65X2!$F$3:$F$94</c:f>
+              <c:f>IXTK102N65X2!#REF!</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="92"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.82764101964858128</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.6534462395073035</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8.4909450910800359</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="0.0">
-                  <c:v>12.583047120130047</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="0.0">
-                  <c:v>16.47116797429733</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="0.0">
-                  <c:v>20.326083377421938</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="0.0">
-                  <c:v>24.166272143329934</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="0.0">
-                  <c:v>28.019478024333566</c:v>
-                </c:pt>
-                <c:pt idx="8" formatCode="0.0">
-                  <c:v>31.766421754415916</c:v>
-                </c:pt>
-                <c:pt idx="9" formatCode="0.0">
-                  <c:v>35.87707897479271</c:v>
-                </c:pt>
-                <c:pt idx="10" formatCode="0.0">
-                  <c:v>39.466477977598117</c:v>
-                </c:pt>
-                <c:pt idx="11" formatCode="0.0">
-                  <c:v>43.269076398215475</c:v>
-                </c:pt>
-                <c:pt idx="12" formatCode="0.0">
-                  <c:v>46.92853011606438</c:v>
-                </c:pt>
-                <c:pt idx="13" formatCode="0.0">
-                  <c:v>50.354147410673434</c:v>
-                </c:pt>
-                <c:pt idx="14" formatCode="0.0">
-                  <c:v>53.89215007900944</c:v>
-                </c:pt>
-                <c:pt idx="15" formatCode="0.0">
-                  <c:v>57.280946563595151</c:v>
-                </c:pt>
-                <c:pt idx="16" formatCode="0.0">
-                  <c:v>60.50949774343708</c:v>
-                </c:pt>
-                <c:pt idx="17" formatCode="0.0">
-                  <c:v>63.808129536553629</c:v>
-                </c:pt>
-                <c:pt idx="18" formatCode="0.0">
-                  <c:v>65.953934522002655</c:v>
-                </c:pt>
-                <c:pt idx="19" formatCode="0.0">
-                  <c:v>62.381958357659499</c:v>
-                </c:pt>
-                <c:pt idx="20" formatCode="0.0">
-                  <c:v>59.209167048388856</c:v>
-                </c:pt>
-                <c:pt idx="21" formatCode="0.0">
-                  <c:v>56.343496267938185</c:v>
-                </c:pt>
-                <c:pt idx="22" formatCode="0.0">
-                  <c:v>53.742411568068867</c:v>
-                </c:pt>
-                <c:pt idx="23" formatCode="0.0">
-                  <c:v>51.370886278235545</c:v>
-                </c:pt>
-                <c:pt idx="24" formatCode="0.0">
-                  <c:v>49.199815011600116</c:v>
-                </c:pt>
-                <c:pt idx="25" formatCode="0.0">
-                  <c:v>47.20481315523454</c:v>
-                </c:pt>
-                <c:pt idx="26" formatCode="0.0">
-                  <c:v>45.365297055060537</c:v>
-                </c:pt>
-                <c:pt idx="27" formatCode="0.0">
-                  <c:v>43.663771198984982</c:v>
-                </c:pt>
-                <c:pt idx="28" formatCode="0.0">
-                  <c:v>42.085270015484404</c:v>
-                </c:pt>
-                <c:pt idx="29" formatCode="0.0">
-                  <c:v>40.616916525947921</c:v>
-                </c:pt>
-                <c:pt idx="30" formatCode="0.0">
-                  <c:v>39.247570273776432</c:v>
-                </c:pt>
-                <c:pt idx="31" formatCode="0.0">
-                  <c:v>37.967544148440027</c:v>
-                </c:pt>
-                <c:pt idx="32" formatCode="0.0">
-                  <c:v>36.768374872614658</c:v>
-                </c:pt>
-                <c:pt idx="33" formatCode="0.0">
-                  <c:v>35.642635651361736</c:v>
-                </c:pt>
-                <c:pt idx="34" formatCode="0.0">
-                  <c:v>34.583782215649443</c:v>
-                </c:pt>
-                <c:pt idx="35" formatCode="0.0">
-                  <c:v>33.735762589318313</c:v>
-                </c:pt>
-                <c:pt idx="36" formatCode="0.0">
-                  <c:v>26.02401764944651</c:v>
-                </c:pt>
-                <c:pt idx="37" formatCode="0.0">
-                  <c:v>24.0435528519176</c:v>
-                </c:pt>
-                <c:pt idx="38" formatCode="0.0">
-                  <c:v>22.261035659934503</c:v>
-                </c:pt>
-                <c:pt idx="39" formatCode="0.0">
-                  <c:v>20.610668968307333</c:v>
-                </c:pt>
-                <c:pt idx="40" formatCode="0.0">
-                  <c:v>19.082655533664276</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>17.667924450993389</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>16.358077305086137</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>15.145338314152067</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>14.022508169636902</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>12.982921298218784</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>12.020406292272279</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>11.129249273899747</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>10.304159975043921</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>9.5402403323196054</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>8.8329554101308307</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>8.1781064794611424</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>7.5718060925220607</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>7.0104550052926013</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>6.4907208109527863</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>6.0095181573706205</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>5.5639904312054158</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>5.1514927998970652</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>4.7695765108715324</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>4.4159743547563517</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>4.0885872063099509</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>3.7854715631662019</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>3.5048280084193122</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>3.2449905285581346</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>3.0044166233369713</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>2.7816781488710052</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>2.5932862526397806</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>2.4075869692265659</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>2.2290956626267362</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>2.0638371683568182</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>1.91083044523618</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>1.769167183547026</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>1.6380064129409713</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>1.5165695100993439</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>1.4041355765106209</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>1.300037158925647</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>1.203656287085527</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>1.1144208052005193</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>1.0318009754021482</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>0.95530633300521173</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>0.86429450919459005</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>0.76337281522955247</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>0.6794182695875215</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>0.60469691327754749</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>0.53840446288357602</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>0.47900363967956822</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>0.42632357021955675</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>0.37958605013304503</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>0.33923104342632693</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>0.31125786554921364</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>0.28067652277033595</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>0.22422064894203664</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4162,7 +4498,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-3663-4392-BE33-75603037D070}"/>
+              <c16:uniqueId val="{00000000-1536-4F8B-87A2-8EF3FC157147}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -8896,7 +9232,7 @@
   <dimension ref="A1:M98"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.7109375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8971,19 +9307,19 @@
         <v>2.3412337734807481E-2</v>
       </c>
       <c r="D3" s="22">
-        <f t="shared" ref="D3:D34" si="0">IF($B3&lt;$K$10/$A3,$B3,$K$10/$A3)</f>
+        <f>IF($B3&lt;$K$10/$A3,$B3,$K$10/$A3)</f>
         <v>0.82764101964858128</v>
       </c>
       <c r="E3" s="15">
-        <f t="shared" ref="E3:E34" si="1">IF($D3=$B3,$C3,$K$10)</f>
+        <f>IF($D3=$B3,$C3,$K$10)</f>
         <v>2.3412337734807481E-2</v>
       </c>
       <c r="F3" s="22">
-        <f t="shared" ref="F3:F34" si="2">IF($B3&lt;$K$11/$A3,$B3,$K$11/$A3)</f>
+        <f>IF($B3&lt;$K$11/$A3,$B3,$K$11/$A3)</f>
         <v>0.82764101964858128</v>
       </c>
       <c r="G3" s="15">
-        <f t="shared" ref="G3:G34" si="3">IF($D3=$B3,$C3,$K$11)</f>
+        <f>IF($D3=$B3,$C3,$K$11)</f>
         <v>2.3412337734807481E-2</v>
       </c>
       <c r="I3" s="8" t="s">
@@ -9000,7 +9336,7 @@
       </c>
       <c r="M3" s="8">
         <f>M5+K4*K10</f>
-        <v>125</v>
+        <v>124.99999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9011,23 +9347,23 @@
         <v>4.6534462395073035</v>
       </c>
       <c r="C4" s="15">
-        <f t="shared" ref="C4:C66" si="4">A4*B4</f>
+        <f t="shared" ref="C4:C66" si="0">A4*B4</f>
         <v>1.1806179792870639</v>
       </c>
       <c r="D4" s="22">
-        <f t="shared" si="0"/>
+        <f>IF($B4&lt;$K$10/$A4,$B4,$K$10/$A4)</f>
         <v>4.6534462395073035</v>
       </c>
       <c r="E4" s="15">
-        <f t="shared" si="1"/>
+        <f>IF($D4=$B4,$C4,$K$10)</f>
         <v>1.1806179792870639</v>
       </c>
       <c r="F4" s="22">
-        <f t="shared" si="2"/>
+        <f>IF($B4&lt;$K$11/$A4,$B4,$K$11/$A4)</f>
         <v>4.6534462395073035</v>
       </c>
       <c r="G4" s="15">
-        <f t="shared" si="3"/>
+        <f>IF($D4=$B4,$C4,$K$11)</f>
         <v>1.1806179792870639</v>
       </c>
       <c r="J4" s="7" t="s">
@@ -9041,7 +9377,7 @@
       </c>
       <c r="M4" s="8">
         <f>M6+K4*K11</f>
-        <v>125</v>
+        <v>124.99999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9052,23 +9388,23 @@
         <v>8.4909450910800359</v>
       </c>
       <c r="C5" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>3.6929542732293195</v>
       </c>
       <c r="D5" s="22">
-        <f t="shared" si="0"/>
+        <f>IF($B5&lt;$K$10/$A5,$B5,$K$10/$A5)</f>
         <v>8.4909450910800359</v>
       </c>
       <c r="E5" s="15">
-        <f t="shared" si="1"/>
+        <f>IF($D5=$B5,$C5,$K$10)</f>
         <v>3.6929542732293195</v>
       </c>
       <c r="F5" s="22">
-        <f t="shared" si="2"/>
+        <f>IF($B5&lt;$K$11/$A5,$B5,$K$11/$A5)</f>
         <v>8.4909450910800359</v>
       </c>
       <c r="G5" s="15">
-        <f t="shared" si="3"/>
+        <f>IF($D5=$B5,$C5,$K$11)</f>
         <v>3.6929542732293195</v>
       </c>
       <c r="I5" s="8" t="s">
@@ -9085,7 +9421,7 @@
       </c>
       <c r="M5" s="12">
         <f>M7+K6*K10</f>
-        <v>105.47314004989263</v>
+        <v>109.0468709188533</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9096,23 +9432,23 @@
         <v>12.583047120130047</v>
       </c>
       <c r="C6" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>8.364817275867221</v>
       </c>
       <c r="D6" s="18">
-        <f t="shared" si="0"/>
+        <f>IF($B6&lt;$K$10/$A6,$B6,$K$10/$A6)</f>
         <v>12.583047120130047</v>
       </c>
       <c r="E6" s="15">
-        <f t="shared" si="1"/>
+        <f>IF($D6=$B6,$C6,$K$10)</f>
         <v>8.364817275867221</v>
       </c>
       <c r="F6" s="18">
-        <f t="shared" si="2"/>
+        <f>IF($B6&lt;$K$11/$A6,$B6,$K$11/$A6)</f>
         <v>12.583047120130047</v>
       </c>
       <c r="G6" s="15">
-        <f t="shared" si="3"/>
+        <f>IF($D6=$B6,$C6,$K$11)</f>
         <v>8.364817275867221</v>
       </c>
       <c r="I6" s="8" t="s">
@@ -9122,14 +9458,15 @@
         <v>23</v>
       </c>
       <c r="K6" s="2">
-        <v>9.0038130076260103E-2</v>
+        <f>0.12/(17*20/(25.4^2))</f>
+        <v>0.22770352941176467</v>
       </c>
       <c r="L6" s="3" t="s">
         <v>7</v>
       </c>
       <c r="M6" s="12">
         <f>M8+K6*K11</f>
-        <v>92.891956869502621</v>
+        <v>101.53516389727922</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9140,23 +9477,23 @@
         <v>16.47116797429733</v>
       </c>
       <c r="C7" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>14.589651318577648</v>
       </c>
       <c r="D7" s="18">
-        <f t="shared" si="0"/>
+        <f>IF($B7&lt;$K$10/$A7,$B7,$K$10/$A7)</f>
         <v>16.47116797429733</v>
       </c>
       <c r="E7" s="16">
-        <f t="shared" si="1"/>
+        <f>IF($D7=$B7,$C7,$K$10)</f>
         <v>14.589651318577648</v>
       </c>
       <c r="F7" s="18">
-        <f t="shared" si="2"/>
+        <f>IF($B7&lt;$K$11/$A7,$B7,$K$11/$A7)</f>
         <v>16.47116797429733</v>
       </c>
       <c r="G7" s="16">
-        <f t="shared" si="3"/>
+        <f>IF($D7=$B7,$C7,$K$11)</f>
         <v>14.589651318577648</v>
       </c>
       <c r="I7" s="8" t="s">
@@ -9173,7 +9510,7 @@
       </c>
       <c r="M7" s="12">
         <f>K2+K7*K10</f>
-        <v>90.821790415153615</v>
+        <v>78.77533927769862</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9184,23 +9521,23 @@
         <v>20.326083377421938</v>
       </c>
       <c r="C8" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>22.496286100557423</v>
       </c>
       <c r="D8" s="18">
-        <f t="shared" si="0"/>
+        <f>IF($B8&lt;$K$10/$A8,$B8,$K$10/$A8)</f>
         <v>20.326083377421938</v>
       </c>
       <c r="E8" s="16">
-        <f t="shared" si="1"/>
+        <f>IF($D8=$B8,$C8,$K$10)</f>
         <v>22.496286100557423</v>
       </c>
       <c r="F8" s="18">
-        <f t="shared" si="2"/>
+        <f>IF($B8&lt;$K$11/$A8,$B8,$K$11/$A8)</f>
         <v>20.326083377421938</v>
       </c>
       <c r="G8" s="16">
-        <f t="shared" si="3"/>
+        <f>IF($D8=$B8,$C8,$K$11)</f>
         <v>22.496286100557423</v>
       </c>
       <c r="I8" s="8" t="s">
@@ -9217,7 +9554,7 @@
       </c>
       <c r="M8" s="12">
         <f>K2+K8*K11</f>
-        <v>68.800722170520174</v>
+        <v>57.009947250128249</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9228,25 +9565,26 @@
         <v>24.166272143329934</v>
       </c>
       <c r="C9" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>32.300872094965342</v>
       </c>
       <c r="D9" s="18">
-        <f t="shared" si="0"/>
+        <f>IF($B9&lt;$K$10/$A9,$B9,$K$10/$A9)</f>
         <v>24.166272143329934</v>
       </c>
       <c r="E9" s="16">
-        <f t="shared" si="1"/>
+        <f>IF($D9=$B9,$C9,$K$10)</f>
         <v>32.300872094965342</v>
       </c>
       <c r="F9" s="18">
-        <f t="shared" si="2"/>
+        <f>IF($B9&lt;$K$11/$A9,$B9,$K$11/$A9)</f>
         <v>24.166272143329934</v>
       </c>
       <c r="G9" s="16">
-        <f t="shared" si="3"/>
+        <f>IF($D9=$B9,$C9,$K$11)</f>
         <v>32.300872094965342</v>
       </c>
+      <c r="M9" s="12"/>
     </row>
     <row r="10" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14">
@@ -9256,23 +9594,23 @@
         <v>28.019478024333566</v>
       </c>
       <c r="C10" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>43.891108874292428</v>
       </c>
       <c r="D10" s="18">
-        <f t="shared" si="0"/>
+        <f>IF($B10&lt;$K$10/$A10,$B10,$K$10/$A10)</f>
         <v>28.019478024333566</v>
       </c>
       <c r="E10" s="16">
-        <f t="shared" si="1"/>
+        <f>IF($D10=$B10,$C10,$K$10)</f>
         <v>43.891108874292428</v>
       </c>
       <c r="F10" s="18">
-        <f t="shared" si="2"/>
+        <f>IF($B10&lt;$K$11/$A10,$B10,$K$11/$A10)</f>
         <v>28.019478024333566</v>
       </c>
       <c r="G10" s="16">
-        <f t="shared" si="3"/>
+        <f>IF($D10=$B10,$C10,$K$11)</f>
         <v>43.891108874292428</v>
       </c>
       <c r="J10" s="8" t="s">
@@ -9280,7 +9618,7 @@
       </c>
       <c r="K10" s="9">
         <f>($K$3-$K$2)/(SUM(K7,K6,K4))</f>
-        <v>162.72383291756145</v>
+        <v>132.94274234288903</v>
       </c>
       <c r="L10" s="8" t="s">
         <v>3</v>
@@ -9294,23 +9632,23 @@
         <v>31.766421754415916</v>
       </c>
       <c r="C11" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>57.061711835027651</v>
       </c>
       <c r="D11" s="18">
-        <f t="shared" si="0"/>
+        <f>IF($B11&lt;$K$10/$A11,$B11,$K$10/$A11)</f>
         <v>31.766421754415916</v>
       </c>
       <c r="E11" s="16">
-        <f t="shared" si="1"/>
+        <f>IF($D11=$B11,$C11,$K$10)</f>
         <v>57.061711835027651</v>
       </c>
       <c r="F11" s="18">
-        <f t="shared" si="2"/>
+        <f>IF($B11&lt;$K$11/$A11,$B11,$K$11/$A11)</f>
         <v>31.766421754415916</v>
       </c>
       <c r="G11" s="16">
-        <f t="shared" si="3"/>
+        <f>IF($D11=$B11,$C11,$K$11)</f>
         <v>57.061711835027651</v>
       </c>
       <c r="J11" s="8" t="s">
@@ -9318,7 +9656,7 @@
       </c>
       <c r="K11" s="9">
         <f>($K$3-$K$2)/(SUM(K8,K6,K4))</f>
-        <v>267.56702608747815</v>
+        <v>195.54030085600641</v>
       </c>
       <c r="L11" s="8" t="s">
         <v>3</v>
@@ -9332,35 +9670,26 @@
         <v>35.87707897479271</v>
       </c>
       <c r="C12" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>72.05733544713992</v>
       </c>
       <c r="D12" s="18">
-        <f t="shared" si="0"/>
+        <f>IF($B12&lt;$K$10/$A12,$B12,$K$10/$A12)</f>
         <v>35.87707897479271</v>
       </c>
       <c r="E12" s="16">
-        <f t="shared" si="1"/>
+        <f>IF($D12=$B12,$C12,$K$10)</f>
         <v>72.05733544713992</v>
       </c>
       <c r="F12" s="18">
-        <f t="shared" si="2"/>
+        <f>IF($B12&lt;$K$11/$A12,$B12,$K$11/$A12)</f>
         <v>35.87707897479271</v>
       </c>
       <c r="G12" s="16">
-        <f t="shared" si="3"/>
+        <f>IF($D12=$B12,$C12,$K$11)</f>
         <v>72.05733544713992</v>
       </c>
-      <c r="J12" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="K12" s="12">
-        <f>MAX(D3:D94)</f>
-        <v>51.823341619826913</v>
-      </c>
-      <c r="L12" s="8" t="s">
-        <v>42</v>
-      </c>
+      <c r="K12" s="9"/>
     </row>
     <row r="13" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14">
@@ -9370,31 +9699,31 @@
         <v>39.466477977598117</v>
       </c>
       <c r="C13" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>87.639683679000655</v>
       </c>
       <c r="D13" s="18">
-        <f t="shared" si="0"/>
+        <f>IF($B13&lt;$K$10/$A13,$B13,$K$10/$A13)</f>
         <v>39.466477977598117</v>
       </c>
       <c r="E13" s="16">
-        <f t="shared" si="1"/>
+        <f>IF($D13=$B13,$C13,$K$10)</f>
         <v>87.639683679000655</v>
       </c>
       <c r="F13" s="18">
-        <f t="shared" si="2"/>
+        <f>IF($B13&lt;$K$11/$A13,$B13,$K$11/$A13)</f>
         <v>39.466477977598117</v>
       </c>
       <c r="G13" s="16">
-        <f t="shared" si="3"/>
+        <f>IF($D13=$B13,$C13,$K$11)</f>
         <v>87.639683679000655</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K13" s="12">
-        <f>MAX(F3:F94)</f>
-        <v>65.953934522002655</v>
+        <f>MAX(D3:D94)</f>
+        <v>46.92853011606438</v>
       </c>
       <c r="L13" s="8" t="s">
         <v>42</v>
@@ -9408,24 +9737,34 @@
         <v>43.269076398215475</v>
       </c>
       <c r="C14" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>106.02875111287261</v>
       </c>
       <c r="D14" s="18">
-        <f t="shared" si="0"/>
+        <f>IF($B14&lt;$K$10/$A14,$B14,$K$10/$A14)</f>
         <v>43.269076398215475</v>
       </c>
       <c r="E14" s="17">
-        <f t="shared" si="1"/>
+        <f>IF($D14=$B14,$C14,$K$10)</f>
         <v>106.02875111287261</v>
       </c>
       <c r="F14" s="18">
-        <f t="shared" si="2"/>
+        <f>IF($B14&lt;$K$11/$A14,$B14,$K$11/$A14)</f>
         <v>43.269076398215475</v>
       </c>
       <c r="G14" s="17">
-        <f t="shared" si="3"/>
+        <f>IF($D14=$B14,$C14,$K$11)</f>
         <v>106.02875111287261</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="K14" s="12">
+        <f>MAX(F3:F94)</f>
+        <v>57.280946563595151</v>
+      </c>
+      <c r="L14" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9436,25 +9775,26 @@
         <v>46.92853011606438</v>
       </c>
       <c r="C15" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>125.78212962456209</v>
       </c>
       <c r="D15" s="18">
-        <f t="shared" si="0"/>
+        <f>IF($B15&lt;$K$10/$A15,$B15,$K$10/$A15)</f>
         <v>46.92853011606438</v>
       </c>
       <c r="E15" s="17">
-        <f t="shared" si="1"/>
+        <f>IF($D15=$B15,$C15,$K$10)</f>
         <v>125.78212962456209</v>
       </c>
       <c r="F15" s="18">
-        <f t="shared" si="2"/>
+        <f>IF($B15&lt;$K$11/$A15,$B15,$K$11/$A15)</f>
         <v>46.92853011606438</v>
       </c>
       <c r="G15" s="17">
-        <f t="shared" si="3"/>
+        <f>IF($D15=$B15,$C15,$K$11)</f>
         <v>125.78212962456209</v>
       </c>
+      <c r="K15" s="12"/>
     </row>
     <row r="16" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14">
@@ -9464,27 +9804,27 @@
         <v>50.354147410673434</v>
       </c>
       <c r="C16" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>146.53719312097749</v>
       </c>
       <c r="D16" s="18">
-        <f t="shared" si="0"/>
+        <f>IF($B16&lt;$K$10/$A16,$B16,$K$10/$A16)</f>
+        <v>45.682726020188127</v>
+      </c>
+      <c r="E16" s="17">
+        <f>IF($D16=$B16,$C16,$K$10)</f>
+        <v>132.94274234288903</v>
+      </c>
+      <c r="F16" s="18">
+        <f>IF($B16&lt;$K$11/$A16,$B16,$K$11/$A16)</f>
         <v>50.354147410673434</v>
       </c>
-      <c r="E16" s="17">
-        <f t="shared" si="1"/>
-        <v>146.53719312097749</v>
-      </c>
-      <c r="F16" s="18">
-        <f t="shared" si="2"/>
-        <v>50.354147410673434</v>
-      </c>
       <c r="G16" s="17">
-        <f t="shared" si="3"/>
-        <v>146.53719312097749</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <f>IF($D16=$B16,$C16,$K$11)</f>
+        <v>195.54030085600641</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14">
         <v>3.139971831830032</v>
       </c>
@@ -9492,27 +9832,35 @@
         <v>53.89215007900944</v>
       </c>
       <c r="C17" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>169.21983320484628</v>
       </c>
       <c r="D17" s="18">
-        <f t="shared" si="0"/>
-        <v>51.823341619826913</v>
+        <f>IF($B17&lt;$K$10/$A17,$B17,$K$10/$A17)</f>
+        <v>42.33883278672841</v>
       </c>
       <c r="E17" s="17">
-        <f t="shared" si="1"/>
-        <v>162.72383291756145</v>
+        <f>IF($D17=$B17,$C17,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F17" s="18">
-        <f t="shared" si="2"/>
+        <f>IF($B17&lt;$K$11/$A17,$B17,$K$11/$A17)</f>
         <v>53.89215007900944</v>
       </c>
       <c r="G17" s="17">
-        <f t="shared" si="3"/>
-        <v>267.56702608747815</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <f>IF($D17=$B17,$C17,$K$11)</f>
+        <v>195.54030085600641</v>
+      </c>
+      <c r="J17" s="8">
+        <f>17*20/(25.4^2)</f>
+        <v>0.52700105400210806</v>
+      </c>
+      <c r="K17" s="8">
+        <f>0.12/J17</f>
+        <v>0.22770352941176467</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14">
         <v>3.369812112313086</v>
       </c>
@@ -9520,27 +9868,27 @@
         <v>57.280946563595151</v>
       </c>
       <c r="C18" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>193.02602753476157</v>
       </c>
       <c r="D18" s="18">
-        <f t="shared" si="0"/>
-        <v>48.288696073878597</v>
+        <f>IF($B18&lt;$K$10/$A18,$B18,$K$10/$A18)</f>
+        <v>39.451084485430044</v>
       </c>
       <c r="E18" s="17">
-        <f t="shared" si="1"/>
-        <v>162.72383291756145</v>
+        <f>IF($D18=$B18,$C18,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F18" s="18">
-        <f t="shared" si="2"/>
+        <f>IF($B18&lt;$K$11/$A18,$B18,$K$11/$A18)</f>
         <v>57.280946563595151</v>
       </c>
       <c r="G18" s="17">
-        <f t="shared" si="3"/>
-        <v>267.56702608747815</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <f>IF($D18=$B18,$C18,$K$11)</f>
+        <v>195.54030085600641</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14">
         <v>3.5996523927961399</v>
       </c>
@@ -9548,27 +9896,27 @@
         <v>60.50949774343708</v>
       </c>
       <c r="C19" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>217.81315833905592</v>
       </c>
       <c r="D19" s="18">
-        <f t="shared" si="0"/>
-        <v>45.205429625153542</v>
+        <f>IF($B19&lt;$K$10/$A19,$B19,$K$10/$A19)</f>
+        <v>36.932105613570563</v>
       </c>
       <c r="E19" s="17">
-        <f t="shared" si="1"/>
-        <v>162.72383291756145</v>
+        <f>IF($D19=$B19,$C19,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F19" s="18">
-        <f t="shared" si="2"/>
-        <v>60.50949774343708</v>
+        <f>IF($B19&lt;$K$11/$A19,$B19,$K$11/$A19)</f>
+        <v>54.321995436930095</v>
       </c>
       <c r="G19" s="17">
-        <f t="shared" si="3"/>
-        <v>267.56702608747815</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <f>IF($D19=$B19,$C19,$K$11)</f>
+        <v>195.54030085600641</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14">
         <v>3.8294926732791947</v>
       </c>
@@ -9576,27 +9924,27 @@
         <v>63.808129536553629</v>
       </c>
       <c r="C20" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>244.35276455588189</v>
       </c>
       <c r="D20" s="18">
-        <f t="shared" si="0"/>
-        <v>42.492269028999353</v>
+        <f>IF($B20&lt;$K$10/$A20,$B20,$K$10/$A20)</f>
+        <v>34.715497243411662</v>
       </c>
       <c r="E20" s="17">
-        <f t="shared" si="1"/>
-        <v>162.72383291756145</v>
+        <f>IF($D20=$B20,$C20,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F20" s="18">
-        <f t="shared" si="2"/>
-        <v>63.808129536553629</v>
+        <f>IF($B20&lt;$K$11/$A20,$B20,$K$11/$A20)</f>
+        <v>51.061672534436589</v>
       </c>
       <c r="G20" s="17">
-        <f t="shared" si="3"/>
-        <v>267.56702608747815</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <f>IF($D20=$B20,$C20,$K$11)</f>
+        <v>195.54030085600641</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14">
         <v>4.0568773952100781</v>
       </c>
@@ -9604,27 +9952,27 @@
         <v>66.809346044065734</v>
       </c>
       <c r="C21" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>271.03732575493814</v>
       </c>
       <c r="D21" s="18">
-        <f t="shared" si="0"/>
-        <v>40.110611454437382</v>
+        <f>IF($B21&lt;$K$10/$A21,$B21,$K$10/$A21)</f>
+        <v>32.769721485754893</v>
       </c>
       <c r="E21" s="17">
-        <f t="shared" si="1"/>
-        <v>162.72383291756145</v>
+        <f>IF($D21=$B21,$C21,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F21" s="18">
-        <f t="shared" si="2"/>
-        <v>65.953934522002655</v>
+        <f>IF($B21&lt;$K$11/$A21,$B21,$K$11/$A21)</f>
+        <v>48.199706771242148</v>
       </c>
       <c r="G21" s="17">
-        <f t="shared" si="3"/>
-        <v>267.56702608747815</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <f>IF($D21=$B21,$C21,$K$11)</f>
+        <v>195.54030085600641</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14">
         <v>4.2891732342453022</v>
       </c>
@@ -9632,27 +9980,27 @@
         <v>69.913261986884748</v>
       </c>
       <c r="C22" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>299.87009203292558</v>
       </c>
       <c r="D22" s="18">
-        <f t="shared" si="0"/>
-        <v>37.938274821439656</v>
+        <f>IF($B22&lt;$K$10/$A22,$B22,$K$10/$A22)</f>
+        <v>30.994957555329627</v>
       </c>
       <c r="E22" s="17">
-        <f t="shared" si="1"/>
-        <v>162.72383291756145</v>
+        <f>IF($D22=$B22,$C22,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F22" s="18">
-        <f t="shared" si="2"/>
-        <v>62.381958357659499</v>
+        <f>IF($B22&lt;$K$11/$A22,$B22,$K$11/$A22)</f>
+        <v>45.589275642864663</v>
       </c>
       <c r="G22" s="17">
-        <f t="shared" si="3"/>
-        <v>267.56702608747815</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <f>IF($D22=$B22,$C22,$K$11)</f>
+        <v>195.54030085600641</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="14">
         <v>4.519013514728357</v>
       </c>
@@ -9660,27 +10008,27 @@
         <v>72.928437640943429</v>
       </c>
       <c r="C23" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>329.56459530744758</v>
       </c>
       <c r="D23" s="18">
-        <f t="shared" si="0"/>
-        <v>36.008706853213063</v>
+        <f>IF($B23&lt;$K$10/$A23,$B23,$K$10/$A23)</f>
+        <v>29.418531701576548</v>
       </c>
       <c r="E23" s="17">
-        <f t="shared" si="1"/>
-        <v>162.72383291756145</v>
+        <f>IF($D23=$B23,$C23,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F23" s="18">
-        <f t="shared" si="2"/>
-        <v>59.209167048388856</v>
+        <f>IF($B23&lt;$K$11/$A23,$B23,$K$11/$A23)</f>
+        <v>43.270572265097677</v>
       </c>
       <c r="G23" s="17">
-        <f t="shared" si="3"/>
-        <v>267.56702608747815</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <f>IF($D23=$B23,$C23,$K$11)</f>
+        <v>195.54030085600641</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="14">
         <v>4.74885379521141</v>
       </c>
@@ -9688,27 +10036,27 @@
         <v>75.823963467460118</v>
       </c>
       <c r="C24" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>360.07691668041929</v>
       </c>
       <c r="D24" s="18">
-        <f t="shared" si="0"/>
-        <v>34.265917616088096</v>
+        <f>IF($B24&lt;$K$10/$A24,$B24,$K$10/$A24)</f>
+        <v>27.994701053324526</v>
       </c>
       <c r="E24" s="17">
-        <f t="shared" si="1"/>
-        <v>162.72383291756145</v>
+        <f>IF($D24=$B24,$C24,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F24" s="18">
-        <f t="shared" si="2"/>
-        <v>56.343496267938185</v>
+        <f>IF($B24&lt;$K$11/$A24,$B24,$K$11/$A24)</f>
+        <v>41.176315230673744</v>
       </c>
       <c r="G24" s="17">
-        <f t="shared" si="3"/>
-        <v>267.56702608747815</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <f>IF($D24=$B24,$C24,$K$11)</f>
+        <v>195.54030085600641</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="14">
         <v>4.9786940756944649</v>
       </c>
@@ -9716,27 +10064,27 @@
         <v>78.902667482332788</v>
       </c>
       <c r="C25" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>392.83224315078053</v>
       </c>
       <c r="D25" s="18">
-        <f t="shared" si="0"/>
-        <v>32.68403931704993</v>
+        <f>IF($B25&lt;$K$10/$A25,$B25,$K$10/$A25)</f>
+        <v>26.702332041629852</v>
       </c>
       <c r="E25" s="17">
-        <f t="shared" si="1"/>
-        <v>162.72383291756145</v>
+        <f>IF($D25=$B25,$C25,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F25" s="18">
-        <f t="shared" si="2"/>
-        <v>53.742411568068867</v>
+        <f>IF($B25&lt;$K$11/$A25,$B25,$K$11/$A25)</f>
+        <v>39.27541999630315</v>
       </c>
       <c r="G25" s="17">
-        <f t="shared" si="3"/>
-        <v>267.56702608747815</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <f>IF($D25=$B25,$C25,$K$11)</f>
+        <v>195.54030085600641</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="14">
         <v>5.2085343561775197</v>
       </c>
@@ -9744,27 +10092,27 @@
         <v>81.432549133491904</v>
       </c>
       <c r="C26" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>424.14422987290646</v>
       </c>
       <c r="D26" s="18">
-        <f t="shared" si="0"/>
-        <v>31.241770100751051</v>
+        <f>IF($B26&lt;$K$10/$A26,$B26,$K$10/$A26)</f>
+        <v>25.524021394850529</v>
       </c>
       <c r="E26" s="17">
-        <f t="shared" si="1"/>
-        <v>162.72383291756145</v>
+        <f>IF($D26=$B26,$C26,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F26" s="18">
-        <f t="shared" si="2"/>
-        <v>51.370886278235545</v>
+        <f>IF($B26&lt;$K$11/$A26,$B26,$K$11/$A26)</f>
+        <v>37.542288767681484</v>
       </c>
       <c r="G26" s="17">
-        <f t="shared" si="3"/>
-        <v>267.56702608747815</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <f>IF($D26=$B26,$C26,$K$11)</f>
+        <v>195.54030085600641</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="14">
         <v>5.4383746366605727</v>
       </c>
@@ -9772,27 +10120,27 @@
         <v>84.193468904023803</v>
       </c>
       <c r="C27" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>457.8756258601137</v>
       </c>
       <c r="D27" s="18">
-        <f t="shared" si="0"/>
-        <v>29.921409205725816</v>
+        <f>IF($B27&lt;$K$10/$A27,$B27,$K$10/$A27)</f>
+        <v>24.445307876862703</v>
       </c>
       <c r="E27" s="17">
-        <f t="shared" si="1"/>
-        <v>162.72383291756145</v>
+        <f>IF($D27=$B27,$C27,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F27" s="18">
-        <f t="shared" si="2"/>
-        <v>49.199815011600116</v>
+        <f>IF($B27&lt;$K$11/$A27,$B27,$K$11/$A27)</f>
+        <v>35.955651075939429</v>
       </c>
       <c r="G27" s="17">
-        <f t="shared" si="3"/>
-        <v>267.56702608747815</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <f>IF($D27=$B27,$C27,$K$11)</f>
+        <v>195.54030085600641</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="14">
         <v>5.6682149171436276</v>
       </c>
@@ -9800,27 +10148,27 @@
         <v>86.780896424619783</v>
       </c>
       <c r="C28" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>491.89277163712597</v>
       </c>
       <c r="D28" s="18">
-        <f t="shared" si="0"/>
-        <v>28.708126861139302</v>
+        <f>IF($B28&lt;$K$10/$A28,$B28,$K$10/$A28)</f>
+        <v>23.454075804500832</v>
       </c>
       <c r="E28" s="17">
-        <f t="shared" si="1"/>
-        <v>162.72383291756145</v>
+        <f>IF($D28=$B28,$C28,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F28" s="18">
-        <f t="shared" si="2"/>
-        <v>47.20481315523454</v>
+        <f>IF($B28&lt;$K$11/$A28,$B28,$K$11/$A28)</f>
+        <v>34.497686434681739</v>
       </c>
       <c r="G28" s="17">
-        <f t="shared" si="3"/>
-        <v>267.56702608747815</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <f>IF($D28=$B28,$C28,$K$11)</f>
+        <v>195.54030085600641</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="14">
         <v>5.8980551976266806</v>
       </c>
@@ -9828,27 +10176,27 @@
         <v>89.482988363276888</v>
       </c>
       <c r="C29" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>527.77560461519306</v>
       </c>
       <c r="D29" s="18">
-        <f t="shared" si="0"/>
-        <v>27.589404891130879</v>
+        <f>IF($B29&lt;$K$10/$A29,$B29,$K$10/$A29)</f>
+        <v>22.540098030344627</v>
       </c>
       <c r="E29" s="17">
-        <f t="shared" si="1"/>
-        <v>162.72383291756145</v>
+        <f>IF($D29=$B29,$C29,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F29" s="18">
-        <f t="shared" si="2"/>
-        <v>45.365297055060537</v>
+        <f>IF($B29&lt;$K$11/$A29,$B29,$K$11/$A29)</f>
+        <v>33.153352131171964</v>
       </c>
       <c r="G29" s="17">
-        <f t="shared" si="3"/>
-        <v>267.56702608747815</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <f>IF($D29=$B29,$C29,$K$11)</f>
+        <v>195.54030085600641</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="14">
         <v>6.1278954781097354</v>
       </c>
@@ -9856,27 +10204,27 @@
         <v>91.779410410458198</v>
       </c>
       <c r="C30" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>562.41463403782438</v>
       </c>
       <c r="D30" s="18">
-        <f t="shared" si="0"/>
-        <v>26.554603207389672</v>
+        <f>IF($B30&lt;$K$10/$A30,$B30,$K$10/$A30)</f>
+        <v>21.694681774157434</v>
       </c>
       <c r="E30" s="17">
-        <f t="shared" si="1"/>
-        <v>162.72383291756145</v>
+        <f>IF($D30=$B30,$C30,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F30" s="18">
-        <f t="shared" si="2"/>
-        <v>43.663771198984982</v>
+        <f>IF($B30&lt;$K$11/$A30,$B30,$K$11/$A30)</f>
+        <v>31.909862293591942</v>
       </c>
       <c r="G30" s="17">
-        <f t="shared" si="3"/>
-        <v>267.56702608747815</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <f>IF($D30=$B30,$C30,$K$11)</f>
+        <v>195.54030085600641</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="14">
         <v>6.3577357585927903</v>
       </c>
@@ -9884,27 +10232,27 @@
         <v>94.384642964914619</v>
       </c>
       <c r="C31" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>600.07261964005113</v>
       </c>
       <c r="D31" s="18">
-        <f t="shared" si="0"/>
-        <v>25.59462033281774</v>
+        <f>IF($B31&lt;$K$10/$A31,$B31,$K$10/$A31)</f>
+        <v>20.91039127620402</v>
       </c>
       <c r="E31" s="17">
-        <f t="shared" si="1"/>
-        <v>162.72383291756145</v>
+        <f>IF($D31=$B31,$C31,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F31" s="18">
-        <f t="shared" si="2"/>
-        <v>42.085270015484404</v>
+        <f>IF($B31&lt;$K$11/$A31,$B31,$K$11/$A31)</f>
+        <v>30.756279952611141</v>
       </c>
       <c r="G31" s="17">
-        <f t="shared" si="3"/>
-        <v>267.56702608747815</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <f>IF($D31=$B31,$C31,$K$11)</f>
+        <v>195.54030085600641</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="14">
         <v>6.5875760390758433</v>
       </c>
@@ -9912,24 +10260,24 @@
         <v>96.876350623477009</v>
       </c>
       <c r="C32" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>638.18032612032732</v>
       </c>
       <c r="D32" s="18">
-        <f t="shared" si="0"/>
-        <v>24.701624991093023</v>
+        <f>IF($B32&lt;$K$10/$A32,$B32,$K$10/$A32)</f>
+        <v>20.180828510260245</v>
       </c>
       <c r="E32" s="17">
-        <f t="shared" si="1"/>
-        <v>162.72383291756145</v>
+        <f>IF($D32=$B32,$C32,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F32" s="18">
-        <f t="shared" si="2"/>
-        <v>40.616916525947921</v>
+        <f>IF($B32&lt;$K$11/$A32,$B32,$K$11/$A32)</f>
+        <v>29.683194500695027</v>
       </c>
       <c r="G32" s="17">
-        <f t="shared" si="3"/>
-        <v>267.56702608747815</v>
+        <f>IF($D32=$B32,$C32,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9940,24 +10288,24 @@
         <v>99.345723647564867</v>
       </c>
       <c r="C33" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>677.28115767329712</v>
       </c>
       <c r="D33" s="18">
-        <f t="shared" si="0"/>
-        <v>23.868841990874635</v>
+        <f>IF($B33&lt;$K$10/$A33,$B33,$K$10/$A33)</f>
+        <v>19.500458254468274</v>
       </c>
       <c r="E33" s="17">
-        <f t="shared" si="1"/>
-        <v>162.72383291756145</v>
+        <f>IF($D33=$B33,$C33,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F33" s="18">
-        <f t="shared" si="2"/>
-        <v>39.247570273776432</v>
+        <f>IF($B33&lt;$K$11/$A33,$B33,$K$11/$A33)</f>
+        <v>28.682464395640473</v>
       </c>
       <c r="G33" s="17">
-        <f t="shared" si="3"/>
-        <v>267.56702608747815</v>
+        <f>IF($D33=$B33,$C33,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9968,24 +10316,24 @@
         <v>101.23771978163613</v>
       </c>
       <c r="C34" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>713.44818890433282</v>
       </c>
       <c r="D34" s="18">
-        <f t="shared" si="0"/>
-        <v>23.090380009235478</v>
+        <f>IF($B34&lt;$K$10/$A34,$B34,$K$10/$A34)</f>
+        <v>18.86446739318356</v>
       </c>
       <c r="E34" s="17">
-        <f t="shared" si="1"/>
-        <v>162.72383291756145</v>
+        <f>IF($D34=$B34,$C34,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F34" s="18">
-        <f t="shared" si="2"/>
-        <v>37.967544148440027</v>
+        <f>IF($B34&lt;$K$11/$A34,$B34,$K$11/$A34)</f>
+        <v>27.747010213143422</v>
       </c>
       <c r="G34" s="17">
-        <f t="shared" si="3"/>
-        <v>267.56702608747815</v>
+        <f>IF($D34=$B34,$C34,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -9996,24 +10344,24 @@
         <v>103.6624900089014</v>
       </c>
       <c r="C35" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>754.36198267123098</v>
       </c>
       <c r="D35" s="18">
-        <f t="shared" ref="D35:D66" si="5">IF($B35&lt;$K$10/$A35,$B35,$K$10/$A35)</f>
-        <v>22.361092010887415</v>
+        <f>IF($B35&lt;$K$10/$A35,$B35,$K$10/$A35)</f>
+        <v>18.268650881737042</v>
       </c>
       <c r="E35" s="17">
-        <f t="shared" ref="E35:E66" si="6">IF($D35=$B35,$C35,$K$10)</f>
-        <v>162.72383291756145</v>
+        <f>IF($D35=$B35,$C35,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F35" s="18">
-        <f t="shared" ref="F35:F66" si="7">IF($B35&lt;$K$11/$A35,$B35,$K$11/$A35)</f>
-        <v>36.768374872614658</v>
+        <f>IF($B35&lt;$K$11/$A35,$B35,$K$11/$A35)</f>
+        <v>26.870646916809928</v>
       </c>
       <c r="G35" s="17">
-        <f t="shared" ref="G35:G66" si="8">IF($D35=$B35,$C35,$K$11)</f>
-        <v>267.56702608747815</v>
+        <f>IF($D35=$B35,$C35,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10024,24 +10372,24 @@
         <v>105.85607018050494</v>
       </c>
       <c r="C36" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>794.65486695630977</v>
       </c>
       <c r="D36" s="18">
-        <f t="shared" si="5"/>
-        <v>21.676461308717052</v>
+        <f>IF($B36&lt;$K$10/$A36,$B36,$K$10/$A36)</f>
+        <v>17.709318659733785</v>
       </c>
       <c r="E36" s="17">
-        <f t="shared" si="6"/>
-        <v>162.72383291756145</v>
+        <f>IF($D36=$B36,$C36,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F36" s="18">
-        <f t="shared" si="7"/>
-        <v>35.642635651361736</v>
+        <f>IF($B36&lt;$K$11/$A36,$B36,$K$11/$A36)</f>
+        <v>26.047946940553381</v>
       </c>
       <c r="G36" s="17">
-        <f t="shared" si="8"/>
-        <v>267.56702608747815</v>
+        <f>IF($D36=$B36,$C36,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10052,24 +10400,24 @@
         <v>108.19382839429662</v>
       </c>
       <c r="C37" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>837.07157082955484</v>
       </c>
       <c r="D37" s="18">
-        <f t="shared" si="5"/>
-        <v>21.032507933458092</v>
+        <f>IF($B37&lt;$K$10/$A37,$B37,$K$10/$A37)</f>
+        <v>17.183219156588134</v>
       </c>
       <c r="E37" s="17">
-        <f t="shared" si="6"/>
-        <v>162.72383291756145</v>
+        <f>IF($D37=$B37,$C37,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F37" s="18">
-        <f t="shared" si="7"/>
-        <v>34.583782215649443</v>
+        <f>IF($B37&lt;$K$11/$A37,$B37,$K$11/$A37)</f>
+        <v>25.274127675866012</v>
       </c>
       <c r="G37" s="17">
-        <f t="shared" si="8"/>
-        <v>267.56702608747815</v>
+        <f>IF($D37=$B37,$C37,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10080,24 +10428,24 @@
         <v>109.80307425998572</v>
       </c>
       <c r="C38" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>870.87647588287609</v>
       </c>
       <c r="D38" s="18">
-        <f t="shared" si="5"/>
-        <v>20.516775460725057</v>
+        <f>IF($B38&lt;$K$10/$A38,$B38,$K$10/$A38)</f>
+        <v>16.761874059123869</v>
       </c>
       <c r="E38" s="17">
-        <f t="shared" si="6"/>
-        <v>162.72383291756145</v>
+        <f>IF($D38=$B38,$C38,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F38" s="18">
-        <f t="shared" si="7"/>
-        <v>33.735762589318313</v>
+        <f>IF($B38&lt;$K$11/$A38,$B38,$K$11/$A38)</f>
+        <v>24.65438758573109</v>
       </c>
       <c r="G38" s="17">
-        <f t="shared" si="8"/>
-        <v>267.56702608747815</v>
+        <f>IF($D38=$B38,$C38,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10108,24 +10456,24 @@
         <v>86.863024185306244</v>
       </c>
       <c r="C39" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>893.08581677515861</v>
       </c>
       <c r="D39" s="18">
-        <f t="shared" si="5"/>
-        <v>15.826792866650564</v>
+        <f>IF($B39&lt;$K$10/$A39,$B39,$K$10/$A39)</f>
+        <v>12.93023405644181</v>
       </c>
       <c r="E39" s="17">
-        <f t="shared" si="6"/>
-        <v>162.72383291756145</v>
+        <f>IF($D39=$B39,$C39,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F39" s="18">
-        <f t="shared" si="7"/>
-        <v>26.02401764944651</v>
+        <f>IF($B39&lt;$K$11/$A39,$B39,$K$11/$A39)</f>
+        <v>19.018577569386601</v>
       </c>
       <c r="G39" s="17">
-        <f t="shared" si="8"/>
-        <v>267.56702608747815</v>
+        <f>IF($D39=$B39,$C39,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10136,24 +10484,24 @@
         <v>91.102378881960576</v>
       </c>
       <c r="C40" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>1013.8265645294078</v>
       </c>
       <c r="D40" s="18">
-        <f t="shared" si="5"/>
-        <v>14.622351394453444</v>
+        <f>IF($B40&lt;$K$10/$A40,$B40,$K$10/$A40)</f>
+        <v>11.946224833978917</v>
       </c>
       <c r="E40" s="17">
-        <f t="shared" si="6"/>
-        <v>162.72383291756145</v>
+        <f>IF($D40=$B40,$C40,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F40" s="18">
-        <f t="shared" si="7"/>
-        <v>24.0435528519176</v>
+        <f>IF($B40&lt;$K$11/$A40,$B40,$K$11/$A40)</f>
+        <v>17.571236736675313</v>
       </c>
       <c r="G40" s="17">
-        <f t="shared" si="8"/>
-        <v>267.56702608747815</v>
+        <f>IF($D40=$B40,$C40,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10164,24 +10512,24 @@
         <v>86.57084582079672</v>
       </c>
       <c r="C41" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>1040.5402567966739</v>
       </c>
       <c r="D41" s="22">
-        <f t="shared" si="5"/>
-        <v>13.538293938038368</v>
+        <f>IF($B41&lt;$K$10/$A41,$B41,$K$10/$A41)</f>
+        <v>11.060567407349287</v>
       </c>
       <c r="E41" s="17">
-        <f t="shared" si="6"/>
-        <v>162.72383291756145</v>
+        <f>IF($D41=$B41,$C41,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F41" s="18">
-        <f t="shared" si="7"/>
-        <v>22.261035659934503</v>
+        <f>IF($B41&lt;$K$11/$A41,$B41,$K$11/$A41)</f>
+        <v>16.268557729107982</v>
       </c>
       <c r="G41" s="17">
-        <f t="shared" si="8"/>
-        <v>267.56702608747815</v>
+        <f>IF($D41=$B41,$C41,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10192,24 +10540,24 @@
         <v>79.134779426321401</v>
       </c>
       <c r="C42" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>1027.3251015650214</v>
       </c>
       <c r="D42" s="22">
-        <f t="shared" si="5"/>
-        <v>12.534605263435964</v>
+        <f>IF($B42&lt;$K$10/$A42,$B42,$K$10/$A42)</f>
+        <v>10.240569976931441</v>
       </c>
       <c r="E42" s="17">
-        <f t="shared" si="6"/>
-        <v>162.72383291756145</v>
+        <f>IF($D42=$B42,$C42,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F42" s="18">
-        <f t="shared" si="7"/>
-        <v>20.610668968307333</v>
+        <f>IF($B42&lt;$K$11/$A42,$B42,$K$11/$A42)</f>
+        <v>15.062455452148036</v>
       </c>
       <c r="G42" s="17">
-        <f t="shared" si="8"/>
-        <v>267.56702608747815</v>
+        <f>IF($D42=$B42,$C42,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10220,24 +10568,24 @@
         <v>73.479760819350034</v>
       </c>
       <c r="C43" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>1030.2948164299542</v>
       </c>
       <c r="D43" s="22">
-        <f t="shared" si="5"/>
-        <v>11.605327069218733</v>
+        <f>IF($B43&lt;$K$10/$A43,$B43,$K$10/$A43)</f>
+        <v>9.4813647067281881</v>
       </c>
       <c r="E43" s="17">
-        <f t="shared" si="6"/>
-        <v>162.72383291756145</v>
+        <f>IF($D43=$B43,$C43,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F43" s="18">
-        <f t="shared" si="7"/>
-        <v>19.082655533664276</v>
+        <f>IF($B43&lt;$K$11/$A43,$B43,$K$11/$A43)</f>
+        <v>13.945769995456384</v>
       </c>
       <c r="G43" s="17">
-        <f t="shared" si="8"/>
-        <v>267.56702608747815</v>
+        <f>IF($D43=$B43,$C43,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10248,24 +10596,24 @@
         <v>68.202093097833327</v>
       </c>
       <c r="C44" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>1032.8678546111025</v>
       </c>
       <c r="D44" s="22">
-        <f t="shared" si="5"/>
-        <v>10.744942784629968</v>
+        <f>IF($B44&lt;$K$10/$A44,$B44,$K$10/$A44)</f>
+        <v>8.7784446475632656</v>
       </c>
       <c r="E44" s="17">
-        <f t="shared" si="6"/>
-        <v>162.72383291756145</v>
+        <f>IF($D44=$B44,$C44,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F44" s="22">
-        <f t="shared" si="7"/>
-        <v>17.667924450993389</v>
+        <f>IF($B44&lt;$K$11/$A44,$B44,$K$11/$A44)</f>
+        <v>12.911872263060292</v>
       </c>
       <c r="G44" s="17">
-        <f t="shared" si="8"/>
-        <v>267.56702608747815</v>
+        <f>IF($D44=$B44,$C44,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10276,24 +10624,24 @@
         <v>63.278664363680953</v>
       </c>
       <c r="C45" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>1035.0412045866437</v>
       </c>
       <c r="D45" s="22">
-        <f t="shared" si="5"/>
-        <v>9.9483448209912382</v>
+        <f>IF($B45&lt;$K$10/$A45,$B45,$K$10/$A45)</f>
+        <v>8.1276369820103938</v>
       </c>
       <c r="E45" s="17">
-        <f t="shared" si="6"/>
-        <v>162.72383291756145</v>
+        <f>IF($D45=$B45,$C45,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F45" s="22">
-        <f t="shared" si="7"/>
-        <v>16.358077305086137</v>
+        <f>IF($B45&lt;$K$11/$A45,$B45,$K$11/$A45)</f>
+        <v>11.954624620361798</v>
       </c>
       <c r="G45" s="17">
-        <f t="shared" si="8"/>
-        <v>267.56702608747815</v>
+        <f>IF($D45=$B45,$C45,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10304,24 +10652,24 @@
         <v>58.802850440691522</v>
       </c>
       <c r="C46" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>1038.8479604434283</v>
       </c>
       <c r="D46" s="22">
-        <f t="shared" si="5"/>
-        <v>9.2108042509927159</v>
+        <f>IF($B46&lt;$K$10/$A46,$B46,$K$10/$A46)</f>
+        <v>7.5250782528633549</v>
       </c>
       <c r="E46" s="17">
-        <f t="shared" si="6"/>
-        <v>162.72383291756145</v>
+        <f>IF($D46=$B46,$C46,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F46" s="22">
-        <f t="shared" si="7"/>
-        <v>15.145338314152067</v>
+        <f>IF($B46&lt;$K$11/$A46,$B46,$K$11/$A46)</f>
+        <v>11.068344458659334</v>
       </c>
       <c r="G46" s="17">
-        <f t="shared" si="8"/>
-        <v>267.56702608747815</v>
+        <f>IF($D46=$B46,$C46,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10332,24 +10680,24 @@
         <v>54.536543721038413</v>
       </c>
       <c r="C47" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>1040.6255885180794</v>
       </c>
       <c r="D47" s="22">
-        <f t="shared" si="5"/>
-        <v>8.5279427358703277</v>
+        <f>IF($B47&lt;$K$10/$A47,$B47,$K$10/$A47)</f>
+        <v>6.9671914280933036</v>
       </c>
       <c r="E47" s="17">
-        <f t="shared" si="6"/>
-        <v>162.72383291756145</v>
+        <f>IF($D47=$B47,$C47,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F47" s="22">
-        <f t="shared" si="7"/>
-        <v>14.022508169636902</v>
+        <f>IF($B47&lt;$K$11/$A47,$B47,$K$11/$A47)</f>
+        <v>10.247770460886878</v>
       </c>
       <c r="G47" s="17">
-        <f t="shared" si="8"/>
-        <v>267.56702608747815</v>
+        <f>IF($D47=$B47,$C47,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10360,24 +10708,24 @@
         <v>49.772760812864334</v>
       </c>
       <c r="C48" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>1025.7744990481156</v>
       </c>
       <c r="D48" s="22">
-        <f t="shared" si="5"/>
-        <v>7.8957065338181902</v>
+        <f>IF($B48&lt;$K$10/$A48,$B48,$K$10/$A48)</f>
+        <v>6.4506646661416864</v>
       </c>
       <c r="E48" s="17">
-        <f t="shared" si="6"/>
-        <v>162.72383291756145</v>
+        <f>IF($D48=$B48,$C48,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F48" s="22">
-        <f t="shared" si="7"/>
-        <v>12.982921298218784</v>
+        <f>IF($B48&lt;$K$11/$A48,$B48,$K$11/$A48)</f>
+        <v>9.4880313683105282</v>
       </c>
       <c r="G48" s="17">
-        <f t="shared" si="8"/>
-        <v>267.56702608747815</v>
+        <f>IF($D48=$B48,$C48,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10388,24 +10736,24 @@
         <v>44.281456098215934</v>
       </c>
       <c r="C49" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>985.6786227467129</v>
       </c>
       <c r="D49" s="22">
-        <f t="shared" si="5"/>
-        <v>7.310342435339634</v>
+        <f>IF($B49&lt;$K$10/$A49,$B49,$K$10/$A49)</f>
+        <v>5.9724316554908308</v>
       </c>
       <c r="E49" s="17">
-        <f t="shared" si="6"/>
-        <v>162.72383291756145</v>
+        <f>IF($D49=$B49,$C49,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F49" s="22">
-        <f t="shared" si="7"/>
-        <v>12.020406292272279</v>
+        <f>IF($B49&lt;$K$11/$A49,$B49,$K$11/$A49)</f>
+        <v>8.7846170627687563</v>
       </c>
       <c r="G49" s="17">
-        <f t="shared" si="8"/>
-        <v>267.56702608747815</v>
+        <f>IF($D49=$B49,$C49,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10416,24 +10764,24 @@
         <v>39.426914645618091</v>
       </c>
       <c r="C50" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>947.8934328727031</v>
       </c>
       <c r="D50" s="22">
-        <f t="shared" si="5"/>
-        <v>6.7683754826795051</v>
+        <f>IF($B50&lt;$K$10/$A50,$B50,$K$10/$A50)</f>
+        <v>5.5296534118001341</v>
       </c>
       <c r="E50" s="17">
-        <f t="shared" si="6"/>
-        <v>162.72383291756145</v>
+        <f>IF($D50=$B50,$C50,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F50" s="22">
-        <f t="shared" si="7"/>
-        <v>11.129249273899747</v>
+        <f>IF($B50&lt;$K$11/$A50,$B50,$K$11/$A50)</f>
+        <v>8.133351792789135</v>
       </c>
       <c r="G50" s="17">
-        <f t="shared" si="8"/>
-        <v>267.56702608747815</v>
+        <f>IF($D50=$B50,$C50,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10444,24 +10792,24 @@
         <v>35.090804374066643</v>
       </c>
       <c r="C51" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>911.1991848075379</v>
       </c>
       <c r="D51" s="22">
-        <f t="shared" si="5"/>
-        <v>6.2665883410711523</v>
+        <f>IF($B51&lt;$K$10/$A51,$B51,$K$10/$A51)</f>
+        <v>5.1197014245481505</v>
       </c>
       <c r="E51" s="17">
-        <f t="shared" si="6"/>
-        <v>162.72383291756145</v>
+        <f>IF($D51=$B51,$C51,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F51" s="22">
-        <f t="shared" si="7"/>
-        <v>10.304159975043921</v>
+        <f>IF($B51&lt;$K$11/$A51,$B51,$K$11/$A51)</f>
+        <v>7.5303693846407116</v>
       </c>
       <c r="G51" s="17">
-        <f t="shared" si="8"/>
-        <v>267.56702608747815</v>
+        <f>IF($D51=$B51,$C51,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10472,24 +10820,24 @@
         <v>31.231572713384239</v>
       </c>
       <c r="C52" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>875.92542114955825</v>
       </c>
       <c r="D52" s="22">
-        <f t="shared" si="5"/>
-        <v>5.8020021993375517</v>
+        <f>IF($B52&lt;$K$10/$A52,$B52,$K$10/$A52)</f>
+        <v>4.7401420531323035</v>
       </c>
       <c r="E52" s="17">
-        <f t="shared" si="6"/>
-        <v>162.72383291756145</v>
+        <f>IF($D52=$B52,$C52,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F52" s="22">
-        <f t="shared" si="7"/>
-        <v>9.5402403323196054</v>
+        <f>IF($B52&lt;$K$11/$A52,$B52,$K$11/$A52)</f>
+        <v>6.9720902911649381</v>
       </c>
       <c r="G52" s="17">
-        <f t="shared" si="8"/>
-        <v>267.56702608747815</v>
+        <f>IF($D52=$B52,$C52,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10500,24 +10848,24 @@
         <v>27.807679785593727</v>
       </c>
       <c r="C53" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>842.34753116612762</v>
       </c>
       <c r="D53" s="22">
-        <f t="shared" si="5"/>
-        <v>5.3718590864648608</v>
+        <f>IF($B53&lt;$K$10/$A53,$B53,$K$10/$A53)</f>
+        <v>4.3887220797951896</v>
       </c>
       <c r="E53" s="17">
-        <f t="shared" si="6"/>
-        <v>162.72383291756145</v>
+        <f>IF($D53=$B53,$C53,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F53" s="22">
-        <f t="shared" si="7"/>
-        <v>8.8329554101308307</v>
+        <f>IF($B53&lt;$K$11/$A53,$B53,$K$11/$A53)</f>
+        <v>6.4552003421377613</v>
       </c>
       <c r="G53" s="17">
-        <f t="shared" si="8"/>
-        <v>267.56702608747815</v>
+        <f>IF($D53=$B53,$C53,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10528,24 +10876,24 @@
         <v>24.749434750948911</v>
       </c>
       <c r="C54" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>809.73910895983101</v>
       </c>
       <c r="D54" s="22">
-        <f t="shared" si="5"/>
-        <v>4.973605499172308</v>
+        <f>IF($B54&lt;$K$10/$A54,$B54,$K$10/$A54)</f>
+        <v>4.0633553336137131</v>
       </c>
       <c r="E54" s="17">
-        <f t="shared" si="6"/>
-        <v>162.72383291756145</v>
+        <f>IF($D54=$B54,$C54,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F54" s="22">
-        <f t="shared" si="7"/>
-        <v>8.1781064794611424</v>
+        <f>IF($B54&lt;$K$11/$A54,$B54,$K$11/$A54)</f>
+        <v>5.976631070016313</v>
       </c>
       <c r="G54" s="17">
-        <f t="shared" si="8"/>
-        <v>267.56702608747815</v>
+        <f>IF($D54=$B54,$C54,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10556,24 +10904,24 @@
         <v>22.027530711455206</v>
       </c>
       <c r="C55" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>778.39300326713817</v>
       </c>
       <c r="D55" s="22">
-        <f t="shared" si="5"/>
-        <v>4.6048772432852303</v>
+        <f>IF($B55&lt;$K$10/$A55,$B55,$K$10/$A55)</f>
+        <v>3.7621103061457775</v>
       </c>
       <c r="E55" s="17">
-        <f t="shared" si="6"/>
-        <v>162.72383291756145</v>
+        <f>IF($D55=$B55,$C55,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F55" s="22">
-        <f t="shared" si="7"/>
-        <v>7.5718060925220607</v>
+        <f>IF($B55&lt;$K$11/$A55,$B55,$K$11/$A55)</f>
+        <v>5.5335414942760623</v>
       </c>
       <c r="G55" s="17">
-        <f t="shared" si="8"/>
-        <v>267.56702608747815</v>
+        <f>IF($D55=$B55,$C55,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10584,24 +10932,24 @@
         <v>19.604977411675986</v>
       </c>
       <c r="C56" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>748.26034809353814</v>
       </c>
       <c r="D56" s="22">
-        <f t="shared" si="5"/>
-        <v>4.2634853989233852</v>
+        <f>IF($B56&lt;$K$10/$A56,$B56,$K$10/$A56)</f>
+        <v>3.4831986852158949</v>
       </c>
       <c r="E56" s="17">
-        <f t="shared" si="6"/>
-        <v>162.72383291756145</v>
+        <f>IF($D56=$B56,$C56,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F56" s="22">
-        <f t="shared" si="7"/>
-        <v>7.0104550052926013</v>
+        <f>IF($B56&lt;$K$11/$A56,$B56,$K$11/$A56)</f>
+        <v>5.1233012562027511</v>
       </c>
       <c r="G56" s="17">
-        <f t="shared" si="8"/>
-        <v>267.56702608747815</v>
+        <f>IF($D56=$B56,$C56,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10612,24 +10960,24 @@
         <v>17.448852726485832</v>
       </c>
       <c r="C57" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>719.29416911384078</v>
       </c>
       <c r="D57" s="22">
-        <f t="shared" si="5"/>
-        <v>3.9474033261882897</v>
+        <f>IF($B57&lt;$K$10/$A57,$B57,$K$10/$A57)</f>
+        <v>3.2249647387716975</v>
       </c>
       <c r="E57" s="17">
-        <f t="shared" si="6"/>
-        <v>162.72383291756145</v>
+        <f>IF($D57=$B57,$C57,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F57" s="22">
-        <f t="shared" si="7"/>
-        <v>6.4907208109527863</v>
+        <f>IF($B57&lt;$K$11/$A57,$B57,$K$11/$A57)</f>
+        <v>4.7434750040204854</v>
       </c>
       <c r="G57" s="17">
-        <f t="shared" si="8"/>
-        <v>267.56702608747815</v>
+        <f>IF($D57=$B57,$C57,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10640,24 +10988,24 @@
         <v>15.529855254475617</v>
       </c>
       <c r="C58" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>691.44931044307214</v>
       </c>
       <c r="D58" s="22">
-        <f t="shared" si="5"/>
-        <v>3.6547546342101116</v>
+        <f>IF($B58&lt;$K$10/$A58,$B58,$K$10/$A58)</f>
+        <v>2.9858754857896308</v>
       </c>
       <c r="E58" s="17">
-        <f t="shared" si="6"/>
-        <v>162.72383291756145</v>
+        <f>IF($D58=$B58,$C58,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F58" s="22">
-        <f t="shared" si="7"/>
-        <v>6.0095181573706205</v>
+        <f>IF($B58&lt;$K$11/$A58,$B58,$K$11/$A58)</f>
+        <v>4.391807935659819</v>
       </c>
       <c r="G58" s="17">
-        <f t="shared" si="8"/>
-        <v>267.56702608747815</v>
+        <f>IF($D58=$B58,$C58,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10668,24 +11016,24 @@
         <v>13.827329350212649</v>
       </c>
       <c r="C59" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>664.94316241427589</v>
       </c>
       <c r="D59" s="22">
-        <f t="shared" si="5"/>
-        <v>3.3838020421334432</v>
+        <f>IF($B59&lt;$K$10/$A59,$B59,$K$10/$A59)</f>
+        <v>2.7645115958803061</v>
       </c>
       <c r="E59" s="17">
-        <f t="shared" si="6"/>
-        <v>162.72383291756145</v>
+        <f>IF($D59=$B59,$C59,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F59" s="22">
-        <f t="shared" si="7"/>
-        <v>5.5639904312054158</v>
+        <f>IF($B59&lt;$K$11/$A59,$B59,$K$11/$A59)</f>
+        <v>4.0662124133417814</v>
       </c>
       <c r="G59" s="17">
-        <f t="shared" si="8"/>
-        <v>267.56702608747815</v>
+        <f>IF($D59=$B59,$C59,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10696,24 +11044,24 @@
         <v>12.296969645499857</v>
       </c>
       <c r="C60" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>638.70099905800737</v>
       </c>
       <c r="D60" s="22">
-        <f t="shared" si="5"/>
-        <v>3.1329370659163636</v>
+        <f>IF($B60&lt;$K$10/$A60,$B60,$K$10/$A60)</f>
+        <v>2.559558963569966</v>
       </c>
       <c r="E60" s="17">
-        <f t="shared" si="6"/>
-        <v>162.72383291756145</v>
+        <f>IF($D60=$B60,$C60,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F60" s="22">
-        <f t="shared" si="7"/>
-        <v>5.1514927998970652</v>
+        <f>IF($B60&lt;$K$11/$A60,$B60,$K$11/$A60)</f>
+        <v>3.7647555705167091</v>
       </c>
       <c r="G60" s="17">
-        <f t="shared" si="8"/>
-        <v>267.56702608747815</v>
+        <f>IF($D60=$B60,$C60,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10724,24 +11072,24 @@
         <v>10.938845130062896</v>
       </c>
       <c r="C61" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>613.6549552378608</v>
       </c>
       <c r="D61" s="22">
-        <f t="shared" si="5"/>
-        <v>2.9006704697193877</v>
+        <f>IF($B61&lt;$K$10/$A61,$B61,$K$10/$A61)</f>
+        <v>2.3698009072395338</v>
       </c>
       <c r="E61" s="17">
-        <f t="shared" si="6"/>
-        <v>162.72383291756145</v>
+        <f>IF($D61=$B61,$C61,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F61" s="22">
-        <f t="shared" si="7"/>
-        <v>4.7695765108715324</v>
+        <f>IF($B61&lt;$K$11/$A61,$B61,$K$11/$A61)</f>
+        <v>3.485647837587591</v>
       </c>
       <c r="G61" s="17">
-        <f t="shared" si="8"/>
-        <v>267.56702608747815</v>
+        <f>IF($D61=$B61,$C61,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10752,24 +11100,24 @@
         <v>9.7523722136697586</v>
       </c>
       <c r="C62" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>590.90316674942426</v>
       </c>
       <c r="D62" s="22">
-        <f t="shared" si="5"/>
-        <v>2.6856234251999176</v>
+        <f>IF($B62&lt;$K$10/$A62,$B62,$K$10/$A62)</f>
+        <v>2.1941109464110218</v>
       </c>
       <c r="E62" s="17">
-        <f t="shared" si="6"/>
-        <v>162.72383291756145</v>
+        <f>IF($D62=$B62,$C62,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F62" s="22">
-        <f t="shared" si="7"/>
-        <v>4.4159743547563517</v>
+        <f>IF($B62&lt;$K$11/$A62,$B62,$K$11/$A62)</f>
+        <v>3.2272323183020073</v>
       </c>
       <c r="G62" s="17">
-        <f t="shared" si="8"/>
-        <v>267.56702608747815</v>
+        <f>IF($D62=$B62,$C62,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10780,24 +11128,24 @@
         <v>8.6730142926167417</v>
       </c>
       <c r="C63" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>567.58301202631412</v>
       </c>
       <c r="D63" s="22">
-        <f t="shared" si="5"/>
-        <v>2.4865193262302197</v>
+        <f>IF($B63&lt;$K$10/$A63,$B63,$K$10/$A63)</f>
+        <v>2.0314461145043676</v>
       </c>
       <c r="E63" s="17">
-        <f t="shared" si="6"/>
-        <v>162.72383291756145</v>
+        <f>IF($D63=$B63,$C63,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F63" s="22">
-        <f t="shared" si="7"/>
-        <v>4.0885872063099509</v>
+        <f>IF($B63&lt;$K$11/$A63,$B63,$K$11/$A63)</f>
+        <v>2.9879749537466695</v>
       </c>
       <c r="G63" s="17">
-        <f t="shared" si="8"/>
-        <v>267.56702608747815</v>
+        <f>IF($D63=$B63,$C63,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10808,24 +11156,24 @@
         <v>7.7282595399286409</v>
       </c>
       <c r="C64" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>546.25358754546801</v>
       </c>
       <c r="D64" s="22">
-        <f t="shared" si="5"/>
-        <v>2.3021762104477217</v>
+        <f>IF($B64&lt;$K$10/$A64,$B64,$K$10/$A64)</f>
+        <v>1.8808407673664738</v>
       </c>
       <c r="E64" s="17">
-        <f t="shared" si="6"/>
-        <v>162.72383291756145</v>
+        <f>IF($D64=$B64,$C64,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F64" s="22">
-        <f t="shared" si="7"/>
-        <v>3.7854715631662019</v>
+        <f>IF($B64&lt;$K$11/$A64,$B64,$K$11/$A64)</f>
+        <v>2.7664554155539762</v>
       </c>
       <c r="G64" s="17">
-        <f t="shared" si="8"/>
-        <v>267.56702608747815</v>
+        <f>IF($D64=$B64,$C64,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10836,24 +11184,24 @@
         <v>6.8783176696731632</v>
       </c>
       <c r="C65" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>525.1073658788273</v>
       </c>
       <c r="D65" s="22">
-        <f t="shared" si="5"/>
-        <v>2.1314997426489843</v>
+        <f>IF($B65&lt;$K$10/$A65,$B65,$K$10/$A65)</f>
+        <v>1.7414008508174508</v>
       </c>
       <c r="E65" s="17">
-        <f t="shared" si="6"/>
-        <v>162.72383291756145</v>
+        <f>IF($D65=$B65,$C65,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F65" s="22">
-        <f t="shared" si="7"/>
-        <v>3.5048280084193122</v>
+        <f>IF($B65&lt;$K$11/$A65,$B65,$K$11/$A65)</f>
+        <v>2.5613586742590888</v>
       </c>
       <c r="G65" s="17">
-        <f t="shared" si="8"/>
-        <v>267.56702608747815</v>
+        <f>IF($D65=$B65,$C65,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10864,24 +11212,24 @@
         <v>6.1170498983431978</v>
       </c>
       <c r="C66" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>504.38386039162145</v>
       </c>
       <c r="D66" s="22">
-        <f t="shared" si="5"/>
-        <v>1.9734767183738373</v>
+        <f>IF($B66&lt;$K$10/$A66,$B66,$K$10/$A66)</f>
+        <v>1.6122985931838196</v>
       </c>
       <c r="E66" s="17">
-        <f t="shared" si="6"/>
-        <v>162.72383291756145</v>
+        <f>IF($D66=$B66,$C66,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F66" s="22">
-        <f t="shared" si="7"/>
-        <v>3.2449905285581346</v>
+        <f>IF($B66&lt;$K$11/$A66,$B66,$K$11/$A66)</f>
+        <v>2.3714671927537787</v>
       </c>
       <c r="G66" s="17">
-        <f t="shared" si="8"/>
-        <v>267.56702608747815</v>
+        <f>IF($D66=$B66,$C66,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10892,24 +11240,24 @@
         <v>5.4485794888347447</v>
       </c>
       <c r="C67" s="17">
-        <f t="shared" ref="C67:C94" si="9">A67*B67</f>
+        <f t="shared" ref="C67:C94" si="1">A67*B67</f>
         <v>485.23903073386538</v>
       </c>
       <c r="D67" s="22">
-        <f t="shared" ref="D67:D94" si="10">IF($B67&lt;$K$10/$A67,$B67,$K$10/$A67)</f>
-        <v>1.8271690491144155</v>
+        <f>IF($B67&lt;$K$10/$A67,$B67,$K$10/$A67)</f>
+        <v>1.4927675913114762</v>
       </c>
       <c r="E67" s="17">
-        <f t="shared" ref="E67:E94" si="11">IF($D67=$B67,$C67,$K$10)</f>
-        <v>162.72383291756145</v>
+        <f>IF($D67=$B67,$C67,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F67" s="22">
-        <f t="shared" ref="F67:F94" si="12">IF($B67&lt;$K$11/$A67,$B67,$K$11/$A67)</f>
-        <v>3.0044166233369713</v>
+        <f>IF($B67&lt;$K$11/$A67,$B67,$K$11/$A67)</f>
+        <v>2.1956536984943225</v>
       </c>
       <c r="G67" s="17">
-        <f t="shared" ref="G67:G94" si="13">IF($D67=$B67,$C67,$K$11)</f>
-        <v>267.56702608747815</v>
+        <f>IF($D67=$B67,$C67,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10920,24 +11268,24 @@
         <v>4.8493532572298674</v>
       </c>
       <c r="C68" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>466.45476580791563</v>
       </c>
       <c r="D68" s="22">
-        <f t="shared" si="10"/>
-        <v>1.6917081934428257</v>
+        <f>IF($B68&lt;$K$10/$A68,$B68,$K$10/$A68)</f>
+        <v>1.3820982608869719</v>
       </c>
       <c r="E68" s="17">
-        <f t="shared" si="11"/>
-        <v>162.72383291756145</v>
+        <f>IF($D68=$B68,$C68,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F68" s="22">
-        <f t="shared" si="12"/>
-        <v>2.7816781488710052</v>
+        <f>IF($B68&lt;$K$11/$A68,$B68,$K$11/$A68)</f>
+        <v>2.0328744915563073</v>
       </c>
       <c r="G68" s="17">
-        <f t="shared" si="13"/>
-        <v>267.56702608747815</v>
+        <f>IF($D68=$B68,$C68,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10948,24 +11296,24 @@
         <v>4.3672370753399798</v>
       </c>
       <c r="C69" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>450.59762888813958</v>
       </c>
       <c r="D69" s="22">
-        <f t="shared" si="10"/>
-        <v>1.5771355874920097</v>
+        <f>IF($B69&lt;$K$10/$A69,$B69,$K$10/$A69)</f>
+        <v>1.2884942929900918</v>
       </c>
       <c r="E69" s="17">
-        <f t="shared" si="11"/>
-        <v>162.72383291756145</v>
+        <f>IF($D69=$B69,$C69,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F69" s="22">
-        <f t="shared" si="12"/>
-        <v>2.5932862526397806</v>
+        <f>IF($B69&lt;$K$11/$A69,$B69,$K$11/$A69)</f>
+        <v>1.8951960615697838</v>
       </c>
       <c r="G69" s="17">
-        <f t="shared" si="13"/>
-        <v>267.56702608747815</v>
+        <f>IF($D69=$B69,$C69,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -10976,24 +11324,24 @@
         <v>3.8975215148596423</v>
       </c>
       <c r="C70" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>433.15080791368916</v>
       </c>
       <c r="D70" s="22">
-        <f t="shared" si="10"/>
-        <v>1.464200523673034</v>
+        <f>IF($B70&lt;$K$10/$A70,$B70,$K$10/$A70)</f>
+        <v>1.1962281705569378</v>
       </c>
       <c r="E70" s="17">
-        <f t="shared" si="11"/>
-        <v>162.72383291756145</v>
+        <f>IF($D70=$B70,$C70,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F70" s="22">
-        <f t="shared" si="12"/>
-        <v>2.4075869692265659</v>
+        <f>IF($B70&lt;$K$11/$A70,$B70,$K$11/$A70)</f>
+        <v>1.7594854163593641</v>
       </c>
       <c r="G70" s="17">
-        <f t="shared" si="13"/>
-        <v>267.56702608747815</v>
+        <f>IF($D70=$B70,$C70,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11004,24 +11352,24 @@
         <v>3.4688782079694396</v>
       </c>
       <c r="C71" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>416.38294916078894</v>
       </c>
       <c r="D71" s="22">
-        <f t="shared" si="10"/>
-        <v>1.3556490703153545</v>
+        <f>IF($B71&lt;$K$10/$A71,$B71,$K$10/$A71)</f>
+        <v>1.1075433870440816</v>
       </c>
       <c r="E71" s="17">
-        <f t="shared" si="11"/>
-        <v>162.72383291756145</v>
+        <f>IF($D71=$B71,$C71,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F71" s="22">
-        <f t="shared" si="12"/>
-        <v>2.2290956626267362</v>
+        <f>IF($B71&lt;$K$11/$A71,$B71,$K$11/$A71)</f>
+        <v>1.6290424230538234</v>
       </c>
       <c r="G71" s="17">
-        <f t="shared" si="13"/>
-        <v>267.56702608747815</v>
+        <f>IF($D71=$B71,$C71,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11032,24 +11380,24 @@
         <v>3.0861655163913486</v>
       </c>
       <c r="C72" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>400.1072089868448</v>
       </c>
       <c r="D72" s="22">
-        <f t="shared" si="10"/>
-        <v>1.2551452974738009</v>
+        <f>IF($B72&lt;$K$10/$A72,$B72,$K$10/$A72)</f>
+        <v>1.0254334284854485</v>
       </c>
       <c r="E72" s="17">
-        <f t="shared" si="11"/>
-        <v>162.72383291756145</v>
+        <f>IF($D72=$B72,$C72,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F72" s="22">
-        <f t="shared" si="12"/>
-        <v>2.0638371683568182</v>
+        <f>IF($B72&lt;$K$11/$A72,$B72,$K$11/$A72)</f>
+        <v>1.5082700836476013</v>
       </c>
       <c r="G72" s="17">
-        <f t="shared" si="13"/>
-        <v>267.56702608747815</v>
+        <f>IF($D72=$B72,$C72,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11060,24 +11408,24 @@
         <v>2.7489097540815175</v>
       </c>
       <c r="C73" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>384.92039401828873</v>
       </c>
       <c r="D73" s="22">
-        <f t="shared" si="10"/>
-        <v>1.1620925741527808</v>
+        <f>IF($B73&lt;$K$10/$A73,$B73,$K$10/$A73)</f>
+        <v>0.94941085699748629</v>
       </c>
       <c r="E73" s="17">
-        <f t="shared" si="11"/>
-        <v>162.72383291756145</v>
+        <f>IF($D73=$B73,$C73,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F73" s="22">
-        <f t="shared" si="12"/>
-        <v>1.91083044523618</v>
+        <f>IF($B73&lt;$K$11/$A73,$B73,$K$11/$A73)</f>
+        <v>1.396451444746186</v>
       </c>
       <c r="G73" s="17">
-        <f t="shared" si="13"/>
-        <v>267.56702608747815</v>
+        <f>IF($D73=$B73,$C73,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11088,24 +11436,24 @@
         <v>2.4456293885521592</v>
       </c>
       <c r="C74" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>369.87447455083606</v>
       </c>
       <c r="D74" s="22">
-        <f t="shared" si="10"/>
-        <v>1.0759385017966225</v>
+        <f>IF($B74&lt;$K$10/$A74,$B74,$K$10/$A74)</f>
+        <v>0.87902437188538896</v>
       </c>
       <c r="E74" s="17">
-        <f t="shared" si="11"/>
-        <v>162.72383291756145</v>
+        <f>IF($D74=$B74,$C74,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F74" s="22">
-        <f t="shared" si="12"/>
-        <v>1.769167183547026</v>
+        <f>IF($B74&lt;$K$11/$A74,$B74,$K$11/$A74)</f>
+        <v>1.2929227057382493</v>
       </c>
       <c r="G74" s="17">
-        <f t="shared" si="13"/>
-        <v>267.56702608747815</v>
+        <f>IF($D74=$B74,$C74,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11116,24 +11464,24 @@
         <v>2.1758091902687622</v>
       </c>
       <c r="C75" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>355.41667589002071</v>
       </c>
       <c r="D75" s="22">
-        <f t="shared" si="10"/>
-        <v>0.99617163502859096</v>
+        <f>IF($B75&lt;$K$10/$A75,$B75,$K$10/$A75)</f>
+        <v>0.81385613053985506</v>
       </c>
       <c r="E75" s="17">
-        <f t="shared" si="11"/>
-        <v>162.72383291756145</v>
+        <f>IF($D75=$B75,$C75,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F75" s="22">
-        <f t="shared" si="12"/>
-        <v>1.6380064129409713</v>
+        <f>IF($B75&lt;$K$11/$A75,$B75,$K$11/$A75)</f>
+        <v>1.1970692782070538</v>
       </c>
       <c r="G75" s="17">
-        <f t="shared" si="13"/>
-        <v>267.56702608747815</v>
+        <f>IF($D75=$B75,$C75,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11144,24 +11492,24 @@
         <v>1.9380370477160003</v>
       </c>
       <c r="C76" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>341.92617341407441</v>
       </c>
       <c r="D76" s="22">
-        <f t="shared" si="10"/>
-        <v>0.92231844550453301</v>
+        <f>IF($B76&lt;$K$10/$A76,$B76,$K$10/$A76)</f>
+        <v>0.75351926795457247</v>
       </c>
       <c r="E76" s="17">
-        <f t="shared" si="11"/>
-        <v>162.72383291756145</v>
+        <f>IF($D76=$B76,$C76,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F76" s="22">
-        <f t="shared" si="12"/>
-        <v>1.5165695100993439</v>
+        <f>IF($B76&lt;$K$11/$A76,$B76,$K$11/$A76)</f>
+        <v>1.1083221374853491</v>
       </c>
       <c r="G76" s="17">
-        <f t="shared" si="13"/>
-        <v>267.56702608747815</v>
+        <f>IF($D76=$B76,$C76,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11172,24 +11520,24 @@
         <v>1.7242182479652839</v>
       </c>
       <c r="C77" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>328.5608289196021</v>
       </c>
       <c r="D77" s="22">
-        <f t="shared" si="10"/>
-        <v>0.85394051085733169</v>
+        <f>IF($B77&lt;$K$10/$A77,$B77,$K$10/$A77)</f>
+        <v>0.69765560013925554</v>
       </c>
       <c r="E77" s="17">
-        <f t="shared" si="11"/>
-        <v>162.72383291756145</v>
+        <f>IF($D77=$B77,$C77,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F77" s="22">
-        <f t="shared" si="12"/>
-        <v>1.4041355765106209</v>
+        <f>IF($B77&lt;$K$11/$A77,$B77,$K$11/$A77)</f>
+        <v>1.0261544446950752</v>
       </c>
       <c r="G77" s="17">
-        <f t="shared" si="13"/>
-        <v>267.56702608747815</v>
+        <f>IF($D77=$B77,$C77,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11200,24 +11548,24 @@
         <v>1.5351935478852345</v>
       </c>
       <c r="C78" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>315.96571625367648</v>
       </c>
       <c r="D78" s="22">
-        <f t="shared" si="10"/>
-        <v>0.79063191204463001</v>
+        <f>IF($B78&lt;$K$10/$A78,$B78,$K$10/$A78)</f>
+        <v>0.64593349779478693</v>
       </c>
       <c r="E78" s="17">
-        <f t="shared" si="11"/>
-        <v>162.72383291756145</v>
+        <f>IF($D78=$B78,$C78,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F78" s="22">
-        <f t="shared" si="12"/>
-        <v>1.300037158925647</v>
+        <f>IF($B78&lt;$K$11/$A78,$B78,$K$11/$A78)</f>
+        <v>0.95007841921895764</v>
       </c>
       <c r="G78" s="17">
-        <f t="shared" si="13"/>
-        <v>267.56702608747815</v>
+        <f>IF($D78=$B78,$C78,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11228,24 +11576,24 @@
         <v>1.3663553678846485</v>
       </c>
       <c r="C79" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>303.73425228291944</v>
       </c>
       <c r="D79" s="22">
-        <f t="shared" si="10"/>
-        <v>0.73201682364942156</v>
+        <f>IF($B79&lt;$K$10/$A79,$B79,$K$10/$A79)</f>
+        <v>0.59804591762773385</v>
       </c>
       <c r="E79" s="17">
-        <f t="shared" si="11"/>
-        <v>162.72383291756145</v>
+        <f>IF($D79=$B79,$C79,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F79" s="22">
-        <f t="shared" si="12"/>
-        <v>1.203656287085527</v>
+        <f>IF($B79&lt;$K$11/$A79,$B79,$K$11/$A79)</f>
+        <v>0.87964244303772343</v>
       </c>
       <c r="G79" s="17">
-        <f t="shared" si="13"/>
-        <v>267.56702608747815</v>
+        <f>IF($D79=$B79,$C79,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11256,24 +11604,24 @@
         <v>1.2156087837889784</v>
       </c>
       <c r="C80" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>291.86176859441287</v>
       </c>
       <c r="D80" s="22">
-        <f t="shared" si="10"/>
-        <v>0.67774728282854824</v>
+        <f>IF($B80&lt;$K$10/$A80,$B80,$K$10/$A80)</f>
+        <v>0.55370857961731856</v>
       </c>
       <c r="E80" s="17">
-        <f t="shared" si="11"/>
-        <v>162.72383291756145</v>
+        <f>IF($D80=$B80,$C80,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F80" s="22">
-        <f t="shared" si="12"/>
-        <v>1.1144208052005193</v>
+        <f>IF($B80&lt;$K$11/$A80,$B80,$K$11/$A80)</f>
+        <v>0.8144283797430919</v>
       </c>
       <c r="G80" s="17">
-        <f t="shared" si="13"/>
-        <v>267.56702608747815</v>
+        <f>IF($D80=$B80,$C80,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11284,24 +11632,24 @@
         <v>1.0716595479507691</v>
       </c>
       <c r="C81" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>277.90316646258276</v>
       </c>
       <c r="D81" s="22">
-        <f t="shared" si="10"/>
-        <v>0.62750112366470556</v>
+        <f>IF($B81&lt;$K$10/$A81,$B81,$K$10/$A81)</f>
+        <v>0.51265827941438114</v>
       </c>
       <c r="E81" s="17">
-        <f t="shared" si="11"/>
-        <v>162.72383291756145</v>
+        <f>IF($D81=$B81,$C81,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F81" s="22">
-        <f t="shared" si="12"/>
-        <v>1.0318009754021482</v>
+        <f>IF($B81&lt;$K$11/$A81,$B81,$K$11/$A81)</f>
+        <v>0.75404909231115091</v>
       </c>
       <c r="G81" s="17">
-        <f t="shared" si="13"/>
-        <v>267.56702608747815</v>
+        <f>IF($D81=$B81,$C81,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11312,24 +11660,24 @@
         <v>0.96817912160374775</v>
       </c>
       <c r="C82" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>271.17250178020998</v>
       </c>
       <c r="D82" s="22">
-        <f t="shared" si="10"/>
-        <v>0.58098006465940732</v>
+        <f>IF($B82&lt;$K$10/$A82,$B82,$K$10/$A82)</f>
+        <v>0.47465132585403252</v>
       </c>
       <c r="E82" s="17">
-        <f t="shared" si="11"/>
-        <v>162.72383291756145</v>
+        <f>IF($D82=$B82,$C82,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F82" s="22">
-        <f t="shared" si="12"/>
-        <v>0.95530633300521173</v>
+        <f>IF($B82&lt;$K$11/$A82,$B82,$K$11/$A82)</f>
+        <v>0.6981461449005858</v>
       </c>
       <c r="G82" s="17">
-        <f t="shared" si="13"/>
-        <v>267.56702608747815</v>
+        <f>IF($D82=$B82,$C82,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11340,24 +11688,24 @@
         <v>0.86429450919459005</v>
       </c>
       <c r="C83" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>262.72160940430302</v>
       </c>
       <c r="D83" s="22">
-        <f t="shared" si="10"/>
-        <v>0.53532450423334965</v>
+        <f>IF($B83&lt;$K$10/$A83,$B83,$K$10/$A83)</f>
+        <v>0.43735147064894686</v>
       </c>
       <c r="E83" s="17">
-        <f t="shared" si="11"/>
-        <v>162.72383291756145</v>
+        <f>IF($D83=$B83,$C83,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F83" s="22">
-        <f t="shared" si="12"/>
-        <v>0.86429450919459005</v>
+        <f>IF($B83&lt;$K$11/$A83,$B83,$K$11/$A83)</f>
+        <v>0.64328324091537969</v>
       </c>
       <c r="G83" s="17">
-        <f t="shared" si="13"/>
-        <v>267.56702608747815</v>
+        <f>IF($D83=$B83,$C83,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11368,24 +11716,24 @@
         <v>0.76337281522955247</v>
       </c>
       <c r="C84" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>249.42109379646976</v>
       </c>
       <c r="D84" s="22">
-        <f t="shared" si="10"/>
-        <v>0.49802905018364718</v>
+        <f>IF($B84&lt;$K$10/$A84,$B84,$K$10/$A84)</f>
+        <v>0.40688168727798524</v>
       </c>
       <c r="E84" s="17">
-        <f t="shared" si="11"/>
-        <v>162.72383291756145</v>
+        <f>IF($D84=$B84,$C84,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F84" s="22">
-        <f t="shared" si="12"/>
-        <v>0.76337281522955247</v>
+        <f>IF($B84&lt;$K$11/$A84,$B84,$K$11/$A84)</f>
+        <v>0.59846642352185853</v>
       </c>
       <c r="G84" s="17">
-        <f t="shared" si="13"/>
-        <v>267.56702608747815</v>
+        <f>IF($D84=$B84,$C84,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11396,24 +11744,24 @@
         <v>0.6794182695875215</v>
       </c>
       <c r="C85" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>239.76566295260889</v>
       </c>
       <c r="D85" s="22">
-        <f t="shared" si="10"/>
-        <v>0.46110666398195194</v>
+        <f>IF($B85&lt;$K$10/$A85,$B85,$K$10/$A85)</f>
+        <v>0.3767166943111383</v>
       </c>
       <c r="E85" s="17">
-        <f t="shared" si="11"/>
-        <v>162.72383291756145</v>
+        <f>IF($D85=$B85,$C85,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F85" s="22">
-        <f t="shared" si="12"/>
-        <v>0.6794182695875215</v>
+        <f>IF($B85&lt;$K$11/$A85,$B85,$K$11/$A85)</f>
+        <v>0.55409791046047541</v>
       </c>
       <c r="G85" s="17">
-        <f t="shared" si="13"/>
-        <v>267.56702608747815</v>
+        <f>IF($D85=$B85,$C85,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11424,24 +11772,24 @@
         <v>0.60469691327754749</v>
       </c>
       <c r="C86" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>230.48400701030704</v>
       </c>
       <c r="D86" s="22">
-        <f t="shared" si="10"/>
-        <v>0.42692159320859291</v>
+        <f>IF($B86&lt;$K$10/$A86,$B86,$K$10/$A86)</f>
+        <v>0.34878804382207018</v>
       </c>
       <c r="E86" s="17">
-        <f t="shared" si="11"/>
-        <v>162.72383291756145</v>
+        <f>IF($D86=$B86,$C86,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F86" s="22">
-        <f t="shared" si="12"/>
-        <v>0.60469691327754749</v>
+        <f>IF($B86&lt;$K$11/$A86,$B86,$K$11/$A86)</f>
+        <v>0.51301874643173118</v>
       </c>
       <c r="G86" s="17">
-        <f t="shared" si="13"/>
-        <v>267.56702608747815</v>
+        <f>IF($D86=$B86,$C86,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11452,24 +11800,24 @@
         <v>0.53840446288357602</v>
       </c>
       <c r="C87" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>221.64858969798016</v>
       </c>
       <c r="D87" s="22">
-        <f t="shared" si="10"/>
-        <v>0.39527090147388755</v>
+        <f>IF($B87&lt;$K$10/$A87,$B87,$K$10/$A87)</f>
+        <v>0.32292994005928061</v>
       </c>
       <c r="E87" s="17">
-        <f t="shared" si="11"/>
-        <v>162.72383291756145</v>
+        <f>IF($D87=$B87,$C87,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F87" s="22">
-        <f t="shared" si="12"/>
-        <v>0.53840446288357602</v>
+        <f>IF($B87&lt;$K$11/$A87,$B87,$K$11/$A87)</f>
+        <v>0.47498506892340669</v>
       </c>
       <c r="G87" s="17">
-        <f t="shared" si="13"/>
-        <v>267.56702608747815</v>
+        <f>IF($D87=$B87,$C87,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="88" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11480,24 +11828,24 @@
         <v>0.47900363967956822</v>
       </c>
       <c r="C88" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>212.98470261250705</v>
       </c>
       <c r="D88" s="22">
-        <f t="shared" si="10"/>
-        <v>0.36596669748592875</v>
+        <f>IF($B88&lt;$K$10/$A88,$B88,$K$10/$A88)</f>
+        <v>0.29898887887306619</v>
       </c>
       <c r="E88" s="17">
-        <f t="shared" si="11"/>
-        <v>162.72383291756145</v>
+        <f>IF($D88=$B88,$C88,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F88" s="22">
-        <f t="shared" si="12"/>
-        <v>0.47900363967956822</v>
+        <f>IF($B88&lt;$K$11/$A88,$B88,$K$11/$A88)</f>
+        <v>0.43977109466154035</v>
       </c>
       <c r="G88" s="17">
-        <f t="shared" si="13"/>
-        <v>267.56702608747815</v>
+        <f>IF($D88=$B88,$C88,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="89" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11508,24 +11856,24 @@
         <v>0.42632357021955675</v>
       </c>
       <c r="C89" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>204.73977418414611</v>
       </c>
       <c r="D89" s="22">
-        <f t="shared" si="10"/>
-        <v>0.33883501965197188</v>
+        <f>IF($B89&lt;$K$10/$A89,$B89,$K$10/$A89)</f>
+        <v>0.27682273645287536</v>
       </c>
       <c r="E89" s="17">
-        <f t="shared" si="11"/>
-        <v>162.72383291756145</v>
+        <f>IF($D89=$B89,$C89,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F89" s="22">
-        <f t="shared" si="12"/>
-        <v>0.42632357021955675</v>
+        <f>IF($B89&lt;$K$11/$A89,$B89,$K$11/$A89)</f>
+        <v>0.40716777926970132</v>
       </c>
       <c r="G89" s="17">
-        <f t="shared" si="13"/>
-        <v>267.56702608747815</v>
+        <f>IF($D89=$B89,$C89,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11536,24 +11884,24 @@
         <v>0.37958605013304503</v>
       </c>
       <c r="C90" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>196.89124113921488</v>
       </c>
       <c r="D90" s="22">
-        <f t="shared" si="10"/>
-        <v>0.31371480337214674</v>
+        <f>IF($B90&lt;$K$10/$A90,$B90,$K$10/$A90)</f>
+        <v>0.2562999256229565</v>
       </c>
       <c r="E90" s="17">
-        <f t="shared" si="11"/>
-        <v>162.72383291756145</v>
+        <f>IF($D90=$B90,$C90,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F90" s="22">
-        <f t="shared" si="12"/>
-        <v>0.37958605013304503</v>
+        <f>IF($B90&lt;$K$11/$A90,$B90,$K$11/$A90)</f>
+        <v>0.37698157629712592</v>
       </c>
       <c r="G90" s="17">
-        <f t="shared" si="13"/>
-        <v>267.56702608747815</v>
+        <f>IF($D90=$B90,$C90,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="91" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11564,24 +11912,24 @@
         <v>0.33923104342632693</v>
       </c>
       <c r="C91" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>190.04875043321539</v>
       </c>
       <c r="D91" s="22">
-        <f t="shared" si="10"/>
-        <v>0.29045692489492958</v>
+        <f>IF($B91&lt;$K$10/$A91,$B91,$K$10/$A91)</f>
+        <v>0.23729861468772706</v>
       </c>
       <c r="E91" s="17">
-        <f t="shared" si="11"/>
-        <v>162.72383291756145</v>
+        <f>IF($D91=$B91,$C91,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F91" s="22">
-        <f t="shared" si="12"/>
+        <f>IF($B91&lt;$K$11/$A91,$B91,$K$11/$A91)</f>
         <v>0.33923104342632693</v>
       </c>
       <c r="G91" s="17">
-        <f t="shared" si="13"/>
-        <v>267.56702608747815</v>
+        <f>IF($D91=$B91,$C91,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="92" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11592,24 +11940,24 @@
         <v>0.31125786554921364</v>
       </c>
       <c r="C92" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>188.34020660716794</v>
       </c>
       <c r="D92" s="22">
-        <f t="shared" si="10"/>
-        <v>0.26892331605831116</v>
+        <f>IF($B92&lt;$K$10/$A92,$B92,$K$10/$A92)</f>
+        <v>0.21970600418961136</v>
       </c>
       <c r="E92" s="17">
-        <f t="shared" si="11"/>
-        <v>162.72383291756145</v>
+        <f>IF($D92=$B92,$C92,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F92" s="22">
-        <f t="shared" si="12"/>
+        <f>IF($B92&lt;$K$11/$A92,$B92,$K$11/$A92)</f>
         <v>0.31125786554921364</v>
       </c>
       <c r="G92" s="17">
-        <f t="shared" si="13"/>
-        <v>267.56702608747815</v>
+        <f>IF($D92=$B92,$C92,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11620,24 +11968,24 @@
         <v>0.28067652277033595</v>
       </c>
       <c r="C93" s="17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>181.24039406240485</v>
       </c>
       <c r="D93" s="22">
-        <f t="shared" si="10"/>
-        <v>0.25200099476409327</v>
+        <f>IF($B93&lt;$K$10/$A93,$B93,$K$10/$A93)</f>
+        <v>0.20588074110844654</v>
       </c>
       <c r="E93" s="17">
-        <f t="shared" si="11"/>
-        <v>162.72383291756145</v>
+        <f>IF($D93=$B93,$C93,$K$10)</f>
+        <v>132.94274234288903</v>
       </c>
       <c r="F93" s="22">
-        <f t="shared" si="12"/>
+        <f>IF($B93&lt;$K$11/$A93,$B93,$K$11/$A93)</f>
         <v>0.28067652277033595</v>
       </c>
       <c r="G93" s="17">
-        <f t="shared" si="13"/>
-        <v>267.56702608747815</v>
+        <f>IF($D93=$B93,$C93,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="94" spans="1:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -11648,24 +11996,24 @@
         <v>0.22422064894203664</v>
       </c>
       <c r="C94" s="21">
-        <f t="shared" si="9"/>
+        <f t="shared" si="1"/>
         <v>147.24563179610752</v>
       </c>
       <c r="D94" s="23">
-        <f t="shared" si="10"/>
+        <f>IF($B94&lt;$K$10/$A94,$B94,$K$10/$A94)</f>
+        <v>0.20244069448207935</v>
+      </c>
+      <c r="E94" s="21">
+        <f>IF($D94=$B94,$C94,$K$10)</f>
+        <v>132.94274234288903</v>
+      </c>
+      <c r="F94" s="23">
+        <f>IF($B94&lt;$K$11/$A94,$B94,$K$11/$A94)</f>
         <v>0.22422064894203664</v>
       </c>
-      <c r="E94" s="21">
-        <f t="shared" si="11"/>
-        <v>147.24563179610752</v>
-      </c>
-      <c r="F94" s="23">
-        <f t="shared" si="12"/>
-        <v>0.22422064894203664</v>
-      </c>
       <c r="G94" s="21">
-        <f t="shared" si="13"/>
-        <v>147.24563179610752</v>
+        <f>IF($D94=$B94,$C94,$K$11)</f>
+        <v>195.54030085600641</v>
       </c>
     </row>
     <row r="95" spans="1:7" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">

</xml_diff>